<commit_message>
Agrega ETL inicial para cargar dimensiones y convocatorias / Ajuste de archivo base
</commit_message>
<xml_diff>
--- a/data_raw/CONVOCATORIAS.xlsx
+++ b/data_raw/CONVOCATORIAS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OmarAndresMontanezMu\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05401364-97A7-42F7-8B1A-3D109E84035C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67F0527-68A8-4CD2-A9ED-52DAEEE0860A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{F7620B14-DF17-479D-BEA2-F7DF27FD67E6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{F7620B14-DF17-479D-BEA2-F7DF27FD67E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Convocatorias" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2166" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2163" uniqueCount="283">
   <si>
     <t>Jugador</t>
   </si>
@@ -1008,7 +1008,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1035,24 +1035,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="42">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1358,6 +1345,12 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1607,10 +1600,10 @@
   <autoFilter ref="A1:E22" xr:uid="{F521FEE5-0A8F-418B-805F-E3C993D16AE3}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{AF93E090-BDE8-453F-85BE-5200E9D12BBC}" name="Fecha"/>
-    <tableColumn id="2" xr3:uid="{CADEF1FD-1F08-41B4-AC35-CE941C62FB3B}" name="Fecha Compromiso" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{CADEF1FD-1F08-41B4-AC35-CE941C62FB3B}" name="Fecha Compromiso" dataDxfId="32"/>
     <tableColumn id="3" xr3:uid="{074B7885-FA33-4D3A-9585-31B3698C1889}" name="Rival"/>
     <tableColumn id="4" xr3:uid="{96273CF3-FD6B-4867-942D-2F4ED093C49D}" name="Condicion"/>
-    <tableColumn id="5" xr3:uid="{3517015F-D8D0-4034-8E1F-BDABFC05A71D}" name="Resultado" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{3517015F-D8D0-4034-8E1F-BDABFC05A71D}" name="Resultado" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1623,7 +1616,7 @@
     <sortCondition ref="A1:A47"/>
   </sortState>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{76EDA5C8-957D-4593-8998-F314A5B81C96}" name="Jugador" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{76EDA5C8-957D-4593-8998-F314A5B81C96}" name="Jugador" dataDxfId="30"/>
     <tableColumn id="2" xr3:uid="{2E02992F-1A4B-41A4-B058-271CC4EACCAB}" name="Edad"/>
     <tableColumn id="4" xr3:uid="{2F921FB1-FA9A-461F-901F-20F402C16277}" name="Altura"/>
     <tableColumn id="5" xr3:uid="{739A5073-A644-4F7B-B841-C03B48F0A1E7}" name="Perfil"/>
@@ -1648,44 +1641,44 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8B76BCE1-9309-4E1A-9A37-E2510B165B1F}" name="Tabla4" displayName="Tabla4" ref="A1:M55" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8B76BCE1-9309-4E1A-9A37-E2510B165B1F}" name="Tabla4" displayName="Tabla4" ref="A1:M55" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="A1:M55" xr:uid="{8B76BCE1-9309-4E1A-9A37-E2510B165B1F}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{F3C45A86-6AA9-4019-B309-A1DE1702F225}" name="Jugador" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{BD67C1D1-FD21-47D2-9326-90E6CFE7FC7E}" name="Diciembre" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{9AF5CF38-B837-4CB6-BC87-04A0F1135D5A}" name="Enero" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{BB14A567-C856-4852-9BC2-08E2BF7ED2A8}" name="Febrero" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{72374A46-24DE-4ED3-ADA9-C800716E966C}" name="Marzo" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{6DB87BE6-8C36-429E-9B47-31D84B501595}" name="Abril" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{57B5AE99-64AA-4ED4-B507-778087B4FE66}" name="Mayo" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{E6F4B822-099F-4D99-8DF4-A86BD4815B9D}" name="Junio" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{217A3ABA-B7DB-4B0D-B1A8-263AA1540AEA}" name="Julio" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{CEB93529-14AC-4C2A-9434-9B913C50FEB6}" name="Agosto" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{EC543C46-05A2-4819-AC75-007F280A4076}" name="Septiembre" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{D6CDBE91-0EED-44BE-9A41-6ACA8059684E}" name="Octubre" dataDxfId="18"/>
-    <tableColumn id="13" xr3:uid="{402A598A-4696-4F59-91A4-9B01EFEB9DCF}" name="Noviembre" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{F3C45A86-6AA9-4019-B309-A1DE1702F225}" name="Jugador" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{BD67C1D1-FD21-47D2-9326-90E6CFE7FC7E}" name="Diciembre" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{9AF5CF38-B837-4CB6-BC87-04A0F1135D5A}" name="Enero" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{BB14A567-C856-4852-9BC2-08E2BF7ED2A8}" name="Febrero" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{72374A46-24DE-4ED3-ADA9-C800716E966C}" name="Marzo" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{6DB87BE6-8C36-429E-9B47-31D84B501595}" name="Abril" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{57B5AE99-64AA-4ED4-B507-778087B4FE66}" name="Mayo" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{E6F4B822-099F-4D99-8DF4-A86BD4815B9D}" name="Junio" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{217A3ABA-B7DB-4B0D-B1A8-263AA1540AEA}" name="Julio" dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{CEB93529-14AC-4C2A-9434-9B913C50FEB6}" name="Agosto" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{EC543C46-05A2-4819-AC75-007F280A4076}" name="Septiembre" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{D6CDBE91-0EED-44BE-9A41-6ACA8059684E}" name="Octubre" dataDxfId="16"/>
+    <tableColumn id="13" xr3:uid="{402A598A-4696-4F59-91A4-9B01EFEB9DCF}" name="Noviembre" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{21C18066-DD4C-472B-ABFE-EECD7336A0DF}" name="Tabla5" displayName="Tabla5" ref="A1:M55" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{21C18066-DD4C-472B-ABFE-EECD7336A0DF}" name="Tabla5" displayName="Tabla5" ref="A1:M55" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:M55" xr:uid="{21C18066-DD4C-472B-ABFE-EECD7336A0DF}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{6F6345C2-5815-443E-A8AC-7ED09E65C93C}" name="Jugador" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{7AAA9E1D-48E6-45FB-B66C-3D9D380C4947}" name="Diciembre" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{E53D2D72-85CC-401B-82CC-8E5AE2A023DB}" name="Enero" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{9CB24DF1-5A4C-42BD-B21F-601440AE81D1}" name="Febrero" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{60753C11-A092-4EB6-9F4B-35CDC5AA99E5}" name="Marzo" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{1B87BC6E-845E-405D-B549-BF15927FCD94}" name="Abril" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{7CB40759-175D-4178-8E80-9BE51F8E8BEA}" name="Mayo" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{A5C3754D-AEA2-4779-834F-193E79516E22}" name="Junio" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{E1B52CE6-C9C2-4DE7-8867-E65C1867AA5C}" name="Julio" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{7D697281-5E75-4C38-84C7-2CBDB3C6D71E}" name="Agosto" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{33DC0F95-D539-4285-8724-73BB030AFAE6}" name="Septiembre" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{61F487E4-E91A-4FC2-8CE5-2D2831B04476}" name="Octubre" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{5876400C-5240-4CE8-82AF-193F0B82C886}" name="Noviembre" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{6F6345C2-5815-443E-A8AC-7ED09E65C93C}" name="Jugador" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{7AAA9E1D-48E6-45FB-B66C-3D9D380C4947}" name="Diciembre" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{E53D2D72-85CC-401B-82CC-8E5AE2A023DB}" name="Enero" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{9CB24DF1-5A4C-42BD-B21F-601440AE81D1}" name="Febrero" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{60753C11-A092-4EB6-9F4B-35CDC5AA99E5}" name="Marzo" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{1B87BC6E-845E-405D-B549-BF15927FCD94}" name="Abril" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{7CB40759-175D-4178-8E80-9BE51F8E8BEA}" name="Mayo" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{A5C3754D-AEA2-4779-834F-193E79516E22}" name="Junio" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{E1B52CE6-C9C2-4DE7-8867-E65C1867AA5C}" name="Julio" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{7D697281-5E75-4C38-84C7-2CBDB3C6D71E}" name="Agosto" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{33DC0F95-D539-4285-8724-73BB030AFAE6}" name="Septiembre" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{61F487E4-E91A-4FC2-8CE5-2D2831B04476}" name="Octubre" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{5876400C-5240-4CE8-82AF-193F0B82C886}" name="Noviembre" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2008,10 +2001,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06AB043B-D6B3-4DBE-BE91-21FE4A8F1517}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:E326"/>
   <sheetViews>
-    <sheetView topLeftCell="A301" workbookViewId="0">
-      <selection activeCell="C314" sqref="C314"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7587,9 +7583,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C69871F6-EAF1-438E-A6CC-F5286B89D3D6}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:AT325"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AT1" sqref="AT1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -50761,2382 +50762,2382 @@
       </c>
     </row>
     <row r="309" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A309" s="12" t="s">
+      <c r="A309" t="s">
         <v>264</v>
       </c>
-      <c r="B309" s="13" t="s">
+      <c r="B309" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C309" s="14">
+      <c r="C309" s="4">
         <v>7</v>
       </c>
-      <c r="D309" s="12">
+      <c r="D309">
         <v>90</v>
       </c>
-      <c r="E309" s="12">
-        <v>0</v>
-      </c>
-      <c r="F309" s="12">
-        <v>0</v>
-      </c>
-      <c r="G309" s="12">
-        <v>0</v>
-      </c>
-      <c r="H309" s="12">
-        <v>0</v>
-      </c>
-      <c r="I309" s="12">
-        <v>0</v>
-      </c>
-      <c r="J309" s="12">
-        <v>0</v>
-      </c>
-      <c r="K309" s="12">
-        <v>0</v>
-      </c>
-      <c r="L309" s="12">
-        <v>0</v>
-      </c>
-      <c r="M309" s="12">
-        <v>0</v>
-      </c>
-      <c r="N309" s="12">
-        <v>0</v>
-      </c>
-      <c r="O309" s="12">
-        <v>0</v>
-      </c>
-      <c r="P309" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q309" s="12">
+      <c r="E309">
+        <v>0</v>
+      </c>
+      <c r="F309">
+        <v>0</v>
+      </c>
+      <c r="G309">
+        <v>0</v>
+      </c>
+      <c r="H309">
+        <v>0</v>
+      </c>
+      <c r="I309">
+        <v>0</v>
+      </c>
+      <c r="J309">
+        <v>0</v>
+      </c>
+      <c r="K309">
+        <v>0</v>
+      </c>
+      <c r="L309">
+        <v>0</v>
+      </c>
+      <c r="M309">
+        <v>0</v>
+      </c>
+      <c r="N309">
+        <v>0</v>
+      </c>
+      <c r="O309">
+        <v>0</v>
+      </c>
+      <c r="P309">
+        <v>0</v>
+      </c>
+      <c r="Q309">
         <v>25</v>
       </c>
-      <c r="R309" s="12">
+      <c r="R309">
         <v>31</v>
       </c>
-      <c r="S309" s="12">
-        <v>3</v>
-      </c>
-      <c r="T309" s="12">
+      <c r="S309">
+        <v>3</v>
+      </c>
+      <c r="T309">
         <v>6</v>
       </c>
-      <c r="U309" s="12">
+      <c r="U309">
         <v>22</v>
       </c>
-      <c r="V309" s="12">
+      <c r="V309">
         <v>25</v>
       </c>
-      <c r="W309" s="12">
-        <v>2</v>
-      </c>
-      <c r="X309" s="12">
+      <c r="W309">
+        <v>2</v>
+      </c>
+      <c r="X309">
         <v>8</v>
       </c>
-      <c r="Y309" s="12">
+      <c r="Y309">
         <v>40</v>
       </c>
-      <c r="Z309" s="12">
-        <v>0</v>
-      </c>
-      <c r="AA309" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB309" s="12">
-        <v>0</v>
-      </c>
-      <c r="AC309" s="12">
-        <v>1</v>
-      </c>
-      <c r="AD309" s="12">
+      <c r="Z309">
+        <v>0</v>
+      </c>
+      <c r="AA309">
+        <v>0</v>
+      </c>
+      <c r="AB309">
+        <v>0</v>
+      </c>
+      <c r="AC309">
+        <v>1</v>
+      </c>
+      <c r="AD309">
         <v>6</v>
       </c>
-      <c r="AE309" s="12">
-        <v>0</v>
-      </c>
-      <c r="AF309" s="12">
-        <v>0</v>
-      </c>
-      <c r="AG309" s="12">
-        <v>0</v>
-      </c>
-      <c r="AH309" s="12">
-        <v>1</v>
-      </c>
-      <c r="AI309" s="12">
+      <c r="AE309">
+        <v>0</v>
+      </c>
+      <c r="AF309">
+        <v>0</v>
+      </c>
+      <c r="AG309">
+        <v>0</v>
+      </c>
+      <c r="AH309">
+        <v>1</v>
+      </c>
+      <c r="AI309">
         <v>8</v>
       </c>
-      <c r="AJ309" s="12">
-        <v>1</v>
-      </c>
-      <c r="AK309" s="12">
-        <v>1</v>
-      </c>
-      <c r="AL309" s="12">
-        <v>0</v>
-      </c>
-      <c r="AM309" s="12">
-        <v>0</v>
-      </c>
-      <c r="AN309" s="12">
-        <v>0</v>
-      </c>
-      <c r="AO309" s="12">
-        <v>0</v>
-      </c>
-      <c r="AP309" s="12">
-        <v>0</v>
-      </c>
-      <c r="AQ309" s="12">
-        <v>0</v>
-      </c>
-      <c r="AR309" s="12">
-        <v>0</v>
-      </c>
-      <c r="AS309" s="12">
-        <v>2</v>
-      </c>
-      <c r="AT309" s="12">
+      <c r="AJ309">
+        <v>1</v>
+      </c>
+      <c r="AK309">
+        <v>1</v>
+      </c>
+      <c r="AL309">
+        <v>0</v>
+      </c>
+      <c r="AM309">
+        <v>0</v>
+      </c>
+      <c r="AN309">
+        <v>0</v>
+      </c>
+      <c r="AO309">
+        <v>0</v>
+      </c>
+      <c r="AP309">
+        <v>0</v>
+      </c>
+      <c r="AQ309">
+        <v>0</v>
+      </c>
+      <c r="AR309">
+        <v>0</v>
+      </c>
+      <c r="AS309">
+        <v>2</v>
+      </c>
+      <c r="AT309">
         <v>0</v>
       </c>
     </row>
     <row r="310" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A310" s="12" t="s">
+      <c r="A310" t="s">
         <v>264</v>
       </c>
-      <c r="B310" s="13" t="s">
+      <c r="B310" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="C310" s="14">
+      <c r="C310" s="4">
         <v>6.8</v>
       </c>
-      <c r="D310" s="12">
+      <c r="D310">
         <v>90</v>
       </c>
-      <c r="E310" s="12">
-        <v>0</v>
-      </c>
-      <c r="F310" s="12">
-        <v>1</v>
-      </c>
-      <c r="G310" s="12">
-        <v>0</v>
-      </c>
-      <c r="H310" s="12">
-        <v>0</v>
-      </c>
-      <c r="I310" s="12">
-        <v>0</v>
-      </c>
-      <c r="J310" s="12">
-        <v>0</v>
-      </c>
-      <c r="K310" s="12">
-        <v>1</v>
-      </c>
-      <c r="L310" s="12">
-        <v>0</v>
-      </c>
-      <c r="M310" s="12">
-        <v>0</v>
-      </c>
-      <c r="N310" s="12">
-        <v>0</v>
-      </c>
-      <c r="O310" s="12">
-        <v>0</v>
-      </c>
-      <c r="P310" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q310" s="12">
+      <c r="E310">
+        <v>0</v>
+      </c>
+      <c r="F310">
+        <v>1</v>
+      </c>
+      <c r="G310">
+        <v>0</v>
+      </c>
+      <c r="H310">
+        <v>0</v>
+      </c>
+      <c r="I310">
+        <v>0</v>
+      </c>
+      <c r="J310">
+        <v>0</v>
+      </c>
+      <c r="K310">
+        <v>1</v>
+      </c>
+      <c r="L310">
+        <v>0</v>
+      </c>
+      <c r="M310">
+        <v>0</v>
+      </c>
+      <c r="N310">
+        <v>0</v>
+      </c>
+      <c r="O310">
+        <v>0</v>
+      </c>
+      <c r="P310">
+        <v>0</v>
+      </c>
+      <c r="Q310">
         <v>43</v>
       </c>
-      <c r="R310" s="12">
+      <c r="R310">
         <v>49</v>
       </c>
-      <c r="S310" s="12">
+      <c r="S310">
         <v>24</v>
       </c>
-      <c r="T310" s="12">
+      <c r="T310">
         <v>28</v>
       </c>
-      <c r="U310" s="12">
+      <c r="U310">
         <v>19</v>
       </c>
-      <c r="V310" s="12">
+      <c r="V310">
         <v>21</v>
       </c>
-      <c r="W310" s="12">
-        <v>1</v>
-      </c>
-      <c r="X310" s="12">
-        <v>3</v>
-      </c>
-      <c r="Y310" s="12">
+      <c r="W310">
+        <v>1</v>
+      </c>
+      <c r="X310">
+        <v>3</v>
+      </c>
+      <c r="Y310">
         <v>62</v>
       </c>
-      <c r="Z310" s="12">
-        <v>0</v>
-      </c>
-      <c r="AA310" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB310" s="12">
-        <v>0</v>
-      </c>
-      <c r="AC310" s="12">
-        <v>1</v>
-      </c>
-      <c r="AD310" s="12">
+      <c r="Z310">
+        <v>0</v>
+      </c>
+      <c r="AA310">
+        <v>0</v>
+      </c>
+      <c r="AB310">
+        <v>0</v>
+      </c>
+      <c r="AC310">
+        <v>1</v>
+      </c>
+      <c r="AD310">
         <v>6</v>
       </c>
-      <c r="AE310" s="12">
-        <v>1</v>
-      </c>
-      <c r="AF310" s="12">
-        <v>2</v>
-      </c>
-      <c r="AG310" s="12">
-        <v>0</v>
-      </c>
-      <c r="AH310" s="12">
-        <v>3</v>
-      </c>
-      <c r="AI310" s="12">
-        <v>2</v>
-      </c>
-      <c r="AJ310" s="12">
-        <v>3</v>
-      </c>
-      <c r="AK310" s="12">
+      <c r="AE310">
+        <v>1</v>
+      </c>
+      <c r="AF310">
+        <v>2</v>
+      </c>
+      <c r="AG310">
+        <v>0</v>
+      </c>
+      <c r="AH310">
+        <v>3</v>
+      </c>
+      <c r="AI310">
+        <v>2</v>
+      </c>
+      <c r="AJ310">
+        <v>3</v>
+      </c>
+      <c r="AK310">
         <v>5</v>
       </c>
-      <c r="AL310" s="12">
-        <v>2</v>
-      </c>
-      <c r="AM310" s="12">
-        <v>3</v>
-      </c>
-      <c r="AN310" s="12">
-        <v>2</v>
-      </c>
-      <c r="AO310" s="12">
-        <v>0</v>
-      </c>
-      <c r="AP310" s="12">
-        <v>0</v>
-      </c>
-      <c r="AQ310" s="12">
-        <v>0</v>
-      </c>
-      <c r="AR310" s="12">
-        <v>0</v>
-      </c>
-      <c r="AS310" s="12">
-        <v>0</v>
-      </c>
-      <c r="AT310" s="12">
+      <c r="AL310">
+        <v>2</v>
+      </c>
+      <c r="AM310">
+        <v>3</v>
+      </c>
+      <c r="AN310">
+        <v>2</v>
+      </c>
+      <c r="AO310">
+        <v>0</v>
+      </c>
+      <c r="AP310">
+        <v>0</v>
+      </c>
+      <c r="AQ310">
+        <v>0</v>
+      </c>
+      <c r="AR310">
+        <v>0</v>
+      </c>
+      <c r="AS310">
+        <v>0</v>
+      </c>
+      <c r="AT310">
         <v>0</v>
       </c>
     </row>
     <row r="311" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A311" s="12" t="s">
+      <c r="A311" t="s">
         <v>264</v>
       </c>
-      <c r="B311" s="13" t="s">
+      <c r="B311" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C311" s="14">
+      <c r="C311" s="4">
         <v>7</v>
       </c>
-      <c r="D311" s="12">
+      <c r="D311">
         <v>45</v>
       </c>
-      <c r="E311" s="12">
-        <v>0</v>
-      </c>
-      <c r="F311" s="12">
-        <v>0</v>
-      </c>
-      <c r="G311" s="12">
-        <v>0</v>
-      </c>
-      <c r="H311" s="12">
-        <v>0</v>
-      </c>
-      <c r="I311" s="12">
-        <v>0</v>
-      </c>
-      <c r="J311" s="12">
-        <v>0</v>
-      </c>
-      <c r="K311" s="12">
-        <v>0</v>
-      </c>
-      <c r="L311" s="12">
-        <v>0</v>
-      </c>
-      <c r="M311" s="12">
-        <v>0</v>
-      </c>
-      <c r="N311" s="12">
-        <v>1</v>
-      </c>
-      <c r="O311" s="12">
-        <v>0</v>
-      </c>
-      <c r="P311" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q311" s="12">
+      <c r="E311">
+        <v>0</v>
+      </c>
+      <c r="F311">
+        <v>0</v>
+      </c>
+      <c r="G311">
+        <v>0</v>
+      </c>
+      <c r="H311">
+        <v>0</v>
+      </c>
+      <c r="I311">
+        <v>0</v>
+      </c>
+      <c r="J311">
+        <v>0</v>
+      </c>
+      <c r="K311">
+        <v>0</v>
+      </c>
+      <c r="L311">
+        <v>0</v>
+      </c>
+      <c r="M311">
+        <v>0</v>
+      </c>
+      <c r="N311">
+        <v>1</v>
+      </c>
+      <c r="O311">
+        <v>0</v>
+      </c>
+      <c r="P311">
+        <v>0</v>
+      </c>
+      <c r="Q311">
         <v>20</v>
       </c>
-      <c r="R311" s="12">
+      <c r="R311">
         <v>20</v>
       </c>
-      <c r="S311" s="12">
+      <c r="S311">
         <v>5</v>
       </c>
-      <c r="T311" s="12">
+      <c r="T311">
         <v>5</v>
       </c>
-      <c r="U311" s="12">
+      <c r="U311">
         <v>15</v>
       </c>
-      <c r="V311" s="12">
+      <c r="V311">
         <v>15</v>
       </c>
-      <c r="W311" s="12">
-        <v>0</v>
-      </c>
-      <c r="X311" s="12">
-        <v>0</v>
-      </c>
-      <c r="Y311" s="12">
+      <c r="W311">
+        <v>0</v>
+      </c>
+      <c r="X311">
+        <v>0</v>
+      </c>
+      <c r="Y311">
         <v>26</v>
       </c>
-      <c r="Z311" s="12">
-        <v>1</v>
-      </c>
-      <c r="AA311" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB311" s="12">
-        <v>0</v>
-      </c>
-      <c r="AC311" s="12">
-        <v>0</v>
-      </c>
-      <c r="AD311" s="12">
-        <v>1</v>
-      </c>
-      <c r="AE311" s="12">
-        <v>0</v>
-      </c>
-      <c r="AF311" s="12">
-        <v>0</v>
-      </c>
-      <c r="AG311" s="12">
-        <v>0</v>
-      </c>
-      <c r="AH311" s="12">
-        <v>1</v>
-      </c>
-      <c r="AI311" s="12">
-        <v>0</v>
-      </c>
-      <c r="AJ311" s="12">
-        <v>0</v>
-      </c>
-      <c r="AK311" s="12">
-        <v>1</v>
-      </c>
-      <c r="AL311" s="12">
-        <v>1</v>
-      </c>
-      <c r="AM311" s="12">
-        <v>1</v>
-      </c>
-      <c r="AN311" s="12">
-        <v>1</v>
-      </c>
-      <c r="AO311" s="12">
-        <v>0</v>
-      </c>
-      <c r="AP311" s="12">
-        <v>0</v>
-      </c>
-      <c r="AQ311" s="12">
-        <v>0</v>
-      </c>
-      <c r="AR311" s="12">
-        <v>0</v>
-      </c>
-      <c r="AS311" s="12">
-        <v>0</v>
-      </c>
-      <c r="AT311" s="12">
+      <c r="Z311">
+        <v>1</v>
+      </c>
+      <c r="AA311">
+        <v>0</v>
+      </c>
+      <c r="AB311">
+        <v>0</v>
+      </c>
+      <c r="AC311">
+        <v>0</v>
+      </c>
+      <c r="AD311">
+        <v>1</v>
+      </c>
+      <c r="AE311">
+        <v>0</v>
+      </c>
+      <c r="AF311">
+        <v>0</v>
+      </c>
+      <c r="AG311">
+        <v>0</v>
+      </c>
+      <c r="AH311">
+        <v>1</v>
+      </c>
+      <c r="AI311">
+        <v>0</v>
+      </c>
+      <c r="AJ311">
+        <v>0</v>
+      </c>
+      <c r="AK311">
+        <v>1</v>
+      </c>
+      <c r="AL311">
+        <v>1</v>
+      </c>
+      <c r="AM311">
+        <v>1</v>
+      </c>
+      <c r="AN311">
+        <v>1</v>
+      </c>
+      <c r="AO311">
+        <v>0</v>
+      </c>
+      <c r="AP311">
+        <v>0</v>
+      </c>
+      <c r="AQ311">
+        <v>0</v>
+      </c>
+      <c r="AR311">
+        <v>0</v>
+      </c>
+      <c r="AS311">
+        <v>0</v>
+      </c>
+      <c r="AT311">
         <v>0</v>
       </c>
     </row>
     <row r="312" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A312" s="12" t="s">
+      <c r="A312" t="s">
         <v>264</v>
       </c>
-      <c r="B312" s="13" t="s">
+      <c r="B312" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C312" s="14">
+      <c r="C312" s="4">
         <v>7.6</v>
       </c>
-      <c r="D312" s="12">
+      <c r="D312">
         <v>90</v>
       </c>
-      <c r="E312" s="12">
-        <v>0</v>
-      </c>
-      <c r="F312" s="12">
-        <v>0</v>
-      </c>
-      <c r="G312" s="12">
-        <v>0</v>
-      </c>
-      <c r="H312" s="12">
-        <v>0</v>
-      </c>
-      <c r="I312" s="12">
-        <v>0</v>
-      </c>
-      <c r="J312" s="12">
-        <v>0</v>
-      </c>
-      <c r="K312" s="12">
-        <v>1</v>
-      </c>
-      <c r="L312" s="12">
-        <v>1</v>
-      </c>
-      <c r="M312" s="12">
-        <v>0</v>
-      </c>
-      <c r="N312" s="12">
-        <v>1</v>
-      </c>
-      <c r="O312" s="12">
-        <v>0</v>
-      </c>
-      <c r="P312" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q312" s="12">
+      <c r="E312">
+        <v>0</v>
+      </c>
+      <c r="F312">
+        <v>0</v>
+      </c>
+      <c r="G312">
+        <v>0</v>
+      </c>
+      <c r="H312">
+        <v>0</v>
+      </c>
+      <c r="I312">
+        <v>0</v>
+      </c>
+      <c r="J312">
+        <v>0</v>
+      </c>
+      <c r="K312">
+        <v>1</v>
+      </c>
+      <c r="L312">
+        <v>1</v>
+      </c>
+      <c r="M312">
+        <v>0</v>
+      </c>
+      <c r="N312">
+        <v>1</v>
+      </c>
+      <c r="O312">
+        <v>0</v>
+      </c>
+      <c r="P312">
+        <v>0</v>
+      </c>
+      <c r="Q312">
         <v>65</v>
       </c>
-      <c r="R312" s="12">
+      <c r="R312">
         <v>71</v>
       </c>
-      <c r="S312" s="12">
+      <c r="S312">
         <v>20</v>
       </c>
-      <c r="T312" s="12">
+      <c r="T312">
         <v>23</v>
       </c>
-      <c r="U312" s="12">
+      <c r="U312">
         <v>45</v>
       </c>
-      <c r="V312" s="12">
+      <c r="V312">
         <v>48</v>
       </c>
-      <c r="W312" s="12">
+      <c r="W312">
         <v>6</v>
       </c>
-      <c r="X312" s="12">
+      <c r="X312">
         <v>10</v>
       </c>
-      <c r="Y312" s="12">
+      <c r="Y312">
         <v>84</v>
       </c>
-      <c r="Z312" s="12">
-        <v>1</v>
-      </c>
-      <c r="AA312" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB312" s="12">
-        <v>0</v>
-      </c>
-      <c r="AC312" s="12">
-        <v>3</v>
-      </c>
-      <c r="AD312" s="12">
+      <c r="Z312">
+        <v>1</v>
+      </c>
+      <c r="AA312">
+        <v>0</v>
+      </c>
+      <c r="AB312">
+        <v>0</v>
+      </c>
+      <c r="AC312">
+        <v>3</v>
+      </c>
+      <c r="AD312">
         <v>8</v>
       </c>
-      <c r="AE312" s="12">
-        <v>0</v>
-      </c>
-      <c r="AF312" s="12">
-        <v>0</v>
-      </c>
-      <c r="AG312" s="12">
-        <v>2</v>
-      </c>
-      <c r="AH312" s="12">
+      <c r="AE312">
+        <v>0</v>
+      </c>
+      <c r="AF312">
+        <v>0</v>
+      </c>
+      <c r="AG312">
+        <v>2</v>
+      </c>
+      <c r="AH312">
         <v>5</v>
       </c>
-      <c r="AI312" s="12">
+      <c r="AI312">
         <v>4</v>
       </c>
-      <c r="AJ312" s="12">
-        <v>3</v>
-      </c>
-      <c r="AK312" s="12">
-        <v>3</v>
-      </c>
-      <c r="AL312" s="12">
-        <v>3</v>
-      </c>
-      <c r="AM312" s="12">
-        <v>3</v>
-      </c>
-      <c r="AN312" s="12">
-        <v>1</v>
-      </c>
-      <c r="AO312" s="12">
-        <v>0</v>
-      </c>
-      <c r="AP312" s="12">
-        <v>0</v>
-      </c>
-      <c r="AQ312" s="12">
-        <v>0</v>
-      </c>
-      <c r="AR312" s="12">
-        <v>0</v>
-      </c>
-      <c r="AS312" s="12">
-        <v>0</v>
-      </c>
-      <c r="AT312" s="12">
+      <c r="AJ312">
+        <v>3</v>
+      </c>
+      <c r="AK312">
+        <v>3</v>
+      </c>
+      <c r="AL312">
+        <v>3</v>
+      </c>
+      <c r="AM312">
+        <v>3</v>
+      </c>
+      <c r="AN312">
+        <v>1</v>
+      </c>
+      <c r="AO312">
+        <v>0</v>
+      </c>
+      <c r="AP312">
+        <v>0</v>
+      </c>
+      <c r="AQ312">
+        <v>0</v>
+      </c>
+      <c r="AR312">
+        <v>0</v>
+      </c>
+      <c r="AS312">
+        <v>0</v>
+      </c>
+      <c r="AT312">
         <v>0</v>
       </c>
     </row>
     <row r="313" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A313" s="12" t="s">
+      <c r="A313" t="s">
         <v>264</v>
       </c>
-      <c r="B313" s="13" t="s">
+      <c r="B313" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C313" s="14">
+      <c r="C313" s="4">
         <v>7.6</v>
       </c>
-      <c r="D313" s="12">
+      <c r="D313">
         <v>90</v>
       </c>
-      <c r="E313" s="12">
-        <v>0</v>
-      </c>
-      <c r="F313" s="12">
-        <v>2</v>
-      </c>
-      <c r="G313" s="12">
-        <v>1</v>
-      </c>
-      <c r="H313" s="12">
-        <v>0</v>
-      </c>
-      <c r="I313" s="12">
-        <v>0</v>
-      </c>
-      <c r="J313" s="12">
-        <v>0</v>
-      </c>
-      <c r="K313" s="12">
-        <v>0</v>
-      </c>
-      <c r="L313" s="12">
-        <v>1</v>
-      </c>
-      <c r="M313" s="12">
-        <v>0</v>
-      </c>
-      <c r="N313" s="12">
-        <v>2</v>
-      </c>
-      <c r="O313" s="12">
-        <v>0</v>
-      </c>
-      <c r="P313" s="12">
-        <v>3</v>
-      </c>
-      <c r="Q313" s="12">
+      <c r="E313">
+        <v>0</v>
+      </c>
+      <c r="F313">
+        <v>2</v>
+      </c>
+      <c r="G313">
+        <v>1</v>
+      </c>
+      <c r="H313">
+        <v>0</v>
+      </c>
+      <c r="I313">
+        <v>0</v>
+      </c>
+      <c r="J313">
+        <v>0</v>
+      </c>
+      <c r="K313">
+        <v>0</v>
+      </c>
+      <c r="L313">
+        <v>1</v>
+      </c>
+      <c r="M313">
+        <v>0</v>
+      </c>
+      <c r="N313">
+        <v>2</v>
+      </c>
+      <c r="O313">
+        <v>0</v>
+      </c>
+      <c r="P313">
+        <v>3</v>
+      </c>
+      <c r="Q313">
         <v>44</v>
       </c>
-      <c r="R313" s="12">
+      <c r="R313">
         <v>51</v>
       </c>
-      <c r="S313" s="12">
+      <c r="S313">
         <v>23</v>
       </c>
-      <c r="T313" s="12">
+      <c r="T313">
         <v>29</v>
       </c>
-      <c r="U313" s="12">
+      <c r="U313">
         <v>18</v>
       </c>
-      <c r="V313" s="12">
+      <c r="V313">
         <v>22</v>
       </c>
-      <c r="W313" s="12">
-        <v>0</v>
-      </c>
-      <c r="X313" s="12">
-        <v>0</v>
-      </c>
-      <c r="Y313" s="12">
+      <c r="W313">
+        <v>0</v>
+      </c>
+      <c r="X313">
+        <v>0</v>
+      </c>
+      <c r="Y313">
         <v>75</v>
       </c>
-      <c r="Z313" s="12">
-        <v>0</v>
-      </c>
-      <c r="AA313" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB313" s="12">
-        <v>0</v>
-      </c>
-      <c r="AC313" s="12">
-        <v>1</v>
-      </c>
-      <c r="AD313" s="12">
+      <c r="Z313">
+        <v>0</v>
+      </c>
+      <c r="AA313">
+        <v>0</v>
+      </c>
+      <c r="AB313">
+        <v>0</v>
+      </c>
+      <c r="AC313">
+        <v>1</v>
+      </c>
+      <c r="AD313">
         <v>13</v>
       </c>
-      <c r="AE313" s="12">
-        <v>2</v>
-      </c>
-      <c r="AF313" s="12">
-        <v>2</v>
-      </c>
-      <c r="AG313" s="12">
-        <v>1</v>
-      </c>
-      <c r="AH313" s="12">
-        <v>2</v>
-      </c>
-      <c r="AI313" s="12">
+      <c r="AE313">
+        <v>2</v>
+      </c>
+      <c r="AF313">
+        <v>2</v>
+      </c>
+      <c r="AG313">
+        <v>1</v>
+      </c>
+      <c r="AH313">
+        <v>2</v>
+      </c>
+      <c r="AI313">
         <v>5</v>
       </c>
-      <c r="AJ313" s="12">
-        <v>3</v>
-      </c>
-      <c r="AK313" s="12">
+      <c r="AJ313">
+        <v>3</v>
+      </c>
+      <c r="AK313">
         <v>6</v>
       </c>
-      <c r="AL313" s="12">
-        <v>1</v>
-      </c>
-      <c r="AM313" s="12">
-        <v>1</v>
-      </c>
-      <c r="AN313" s="12">
-        <v>1</v>
-      </c>
-      <c r="AO313" s="12">
-        <v>1</v>
-      </c>
-      <c r="AP313" s="12">
-        <v>0</v>
-      </c>
-      <c r="AQ313" s="12">
-        <v>0</v>
-      </c>
-      <c r="AR313" s="12">
-        <v>0</v>
-      </c>
-      <c r="AS313" s="12">
-        <v>0</v>
-      </c>
-      <c r="AT313" s="12">
+      <c r="AL313">
+        <v>1</v>
+      </c>
+      <c r="AM313">
+        <v>1</v>
+      </c>
+      <c r="AN313">
+        <v>1</v>
+      </c>
+      <c r="AO313">
+        <v>1</v>
+      </c>
+      <c r="AP313">
+        <v>0</v>
+      </c>
+      <c r="AQ313">
+        <v>0</v>
+      </c>
+      <c r="AR313">
+        <v>0</v>
+      </c>
+      <c r="AS313">
+        <v>0</v>
+      </c>
+      <c r="AT313">
         <v>0</v>
       </c>
     </row>
     <row r="314" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A314" s="12" t="s">
+      <c r="A314" t="s">
         <v>264</v>
       </c>
-      <c r="B314" s="13" t="s">
+      <c r="B314" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C314" s="14">
+      <c r="C314" s="4">
         <v>6.7</v>
       </c>
-      <c r="D314" s="12">
+      <c r="D314">
         <v>90</v>
       </c>
-      <c r="E314" s="12">
-        <v>0</v>
-      </c>
-      <c r="F314" s="12">
-        <v>1</v>
-      </c>
-      <c r="G314" s="12">
-        <v>1</v>
-      </c>
-      <c r="H314" s="12">
-        <v>0</v>
-      </c>
-      <c r="I314" s="12">
-        <v>0</v>
-      </c>
-      <c r="J314" s="12">
-        <v>0</v>
-      </c>
-      <c r="K314" s="12">
-        <v>0</v>
-      </c>
-      <c r="L314" s="12">
-        <v>0</v>
-      </c>
-      <c r="M314" s="12">
-        <v>0</v>
-      </c>
-      <c r="N314" s="12">
-        <v>1</v>
-      </c>
-      <c r="O314" s="12">
-        <v>0</v>
-      </c>
-      <c r="P314" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q314" s="12">
+      <c r="E314">
+        <v>0</v>
+      </c>
+      <c r="F314">
+        <v>1</v>
+      </c>
+      <c r="G314">
+        <v>1</v>
+      </c>
+      <c r="H314">
+        <v>0</v>
+      </c>
+      <c r="I314">
+        <v>0</v>
+      </c>
+      <c r="J314">
+        <v>0</v>
+      </c>
+      <c r="K314">
+        <v>0</v>
+      </c>
+      <c r="L314">
+        <v>0</v>
+      </c>
+      <c r="M314">
+        <v>0</v>
+      </c>
+      <c r="N314">
+        <v>1</v>
+      </c>
+      <c r="O314">
+        <v>0</v>
+      </c>
+      <c r="P314">
+        <v>0</v>
+      </c>
+      <c r="Q314">
         <v>46</v>
       </c>
-      <c r="R314" s="12">
+      <c r="R314">
         <v>53</v>
       </c>
-      <c r="S314" s="12">
+      <c r="S314">
         <v>27</v>
       </c>
-      <c r="T314" s="12">
+      <c r="T314">
         <v>33</v>
       </c>
-      <c r="U314" s="12">
+      <c r="U314">
         <v>19</v>
       </c>
-      <c r="V314" s="12">
+      <c r="V314">
         <v>20</v>
       </c>
-      <c r="W314" s="12">
-        <v>0</v>
-      </c>
-      <c r="X314" s="12">
-        <v>0</v>
-      </c>
-      <c r="Y314" s="12">
+      <c r="W314">
+        <v>0</v>
+      </c>
+      <c r="X314">
+        <v>0</v>
+      </c>
+      <c r="Y314">
         <v>65</v>
       </c>
-      <c r="Z314" s="12">
-        <v>1</v>
-      </c>
-      <c r="AA314" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB314" s="12">
-        <v>0</v>
-      </c>
-      <c r="AC314" s="12">
-        <v>0</v>
-      </c>
-      <c r="AD314" s="12">
+      <c r="Z314">
+        <v>1</v>
+      </c>
+      <c r="AA314">
+        <v>0</v>
+      </c>
+      <c r="AB314">
+        <v>0</v>
+      </c>
+      <c r="AC314">
+        <v>0</v>
+      </c>
+      <c r="AD314">
         <v>10</v>
       </c>
-      <c r="AE314" s="12">
-        <v>1</v>
-      </c>
-      <c r="AF314" s="12">
-        <v>1</v>
-      </c>
-      <c r="AG314" s="12">
-        <v>1</v>
-      </c>
-      <c r="AH314" s="12">
-        <v>3</v>
-      </c>
-      <c r="AI314" s="12">
+      <c r="AE314">
+        <v>1</v>
+      </c>
+      <c r="AF314">
+        <v>1</v>
+      </c>
+      <c r="AG314">
+        <v>1</v>
+      </c>
+      <c r="AH314">
+        <v>3</v>
+      </c>
+      <c r="AI314">
         <v>7</v>
       </c>
-      <c r="AJ314" s="12">
-        <v>1</v>
-      </c>
-      <c r="AK314" s="12">
+      <c r="AJ314">
+        <v>1</v>
+      </c>
+      <c r="AK314">
         <v>4</v>
       </c>
-      <c r="AL314" s="12">
-        <v>0</v>
-      </c>
-      <c r="AM314" s="12">
-        <v>0</v>
-      </c>
-      <c r="AN314" s="12">
-        <v>0</v>
-      </c>
-      <c r="AO314" s="12">
-        <v>1</v>
-      </c>
-      <c r="AP314" s="12">
-        <v>0</v>
-      </c>
-      <c r="AQ314" s="12">
-        <v>0</v>
-      </c>
-      <c r="AR314" s="12">
-        <v>0</v>
-      </c>
-      <c r="AS314" s="12">
-        <v>0</v>
-      </c>
-      <c r="AT314" s="12">
+      <c r="AL314">
+        <v>0</v>
+      </c>
+      <c r="AM314">
+        <v>0</v>
+      </c>
+      <c r="AN314">
+        <v>0</v>
+      </c>
+      <c r="AO314">
+        <v>1</v>
+      </c>
+      <c r="AP314">
+        <v>0</v>
+      </c>
+      <c r="AQ314">
+        <v>0</v>
+      </c>
+      <c r="AR314">
+        <v>0</v>
+      </c>
+      <c r="AS314">
+        <v>0</v>
+      </c>
+      <c r="AT314">
         <v>0</v>
       </c>
     </row>
     <row r="315" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A315" s="12" t="s">
+      <c r="A315" t="s">
         <v>264</v>
       </c>
       <c r="B315" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C315" s="14">
+      <c r="C315" s="4">
         <v>8</v>
       </c>
-      <c r="D315" s="12">
+      <c r="D315">
         <v>64</v>
       </c>
-      <c r="E315" s="12">
-        <v>1</v>
-      </c>
-      <c r="F315" s="12">
-        <v>3</v>
-      </c>
-      <c r="G315" s="12">
-        <v>1</v>
-      </c>
-      <c r="H315" s="12">
-        <v>0</v>
-      </c>
-      <c r="I315" s="12">
-        <v>0</v>
-      </c>
-      <c r="J315" s="12">
-        <v>0</v>
-      </c>
-      <c r="K315" s="12">
-        <v>0</v>
-      </c>
-      <c r="L315" s="12">
-        <v>0</v>
-      </c>
-      <c r="M315" s="12">
-        <v>0</v>
-      </c>
-      <c r="N315" s="12">
-        <v>0</v>
-      </c>
-      <c r="O315" s="12">
-        <v>0</v>
-      </c>
-      <c r="P315" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q315" s="12">
+      <c r="E315">
+        <v>1</v>
+      </c>
+      <c r="F315">
+        <v>3</v>
+      </c>
+      <c r="G315">
+        <v>1</v>
+      </c>
+      <c r="H315">
+        <v>0</v>
+      </c>
+      <c r="I315">
+        <v>0</v>
+      </c>
+      <c r="J315">
+        <v>0</v>
+      </c>
+      <c r="K315">
+        <v>0</v>
+      </c>
+      <c r="L315">
+        <v>0</v>
+      </c>
+      <c r="M315">
+        <v>0</v>
+      </c>
+      <c r="N315">
+        <v>0</v>
+      </c>
+      <c r="O315">
+        <v>0</v>
+      </c>
+      <c r="P315">
+        <v>0</v>
+      </c>
+      <c r="Q315">
         <v>45</v>
       </c>
-      <c r="R315" s="12">
+      <c r="R315">
         <v>50</v>
       </c>
-      <c r="S315" s="12">
+      <c r="S315">
         <v>34</v>
       </c>
-      <c r="T315" s="12">
+      <c r="T315">
         <v>38</v>
       </c>
-      <c r="U315" s="12">
+      <c r="U315">
         <v>11</v>
       </c>
-      <c r="V315" s="12">
+      <c r="V315">
         <v>12</v>
       </c>
-      <c r="W315" s="12">
-        <v>2</v>
-      </c>
-      <c r="X315" s="12">
-        <v>2</v>
-      </c>
-      <c r="Y315" s="12">
+      <c r="W315">
+        <v>2</v>
+      </c>
+      <c r="X315">
+        <v>2</v>
+      </c>
+      <c r="Y315">
         <v>65</v>
       </c>
-      <c r="Z315" s="12">
-        <v>1</v>
-      </c>
-      <c r="AA315" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB315" s="12">
-        <v>0</v>
-      </c>
-      <c r="AC315" s="12">
-        <v>2</v>
-      </c>
-      <c r="AD315" s="12">
+      <c r="Z315">
+        <v>1</v>
+      </c>
+      <c r="AA315">
+        <v>0</v>
+      </c>
+      <c r="AB315">
+        <v>0</v>
+      </c>
+      <c r="AC315">
+        <v>2</v>
+      </c>
+      <c r="AD315">
         <v>6</v>
       </c>
-      <c r="AE315" s="12">
-        <v>1</v>
-      </c>
-      <c r="AF315" s="12">
-        <v>1</v>
-      </c>
-      <c r="AG315" s="12">
-        <v>2</v>
-      </c>
-      <c r="AH315" s="12">
-        <v>2</v>
-      </c>
-      <c r="AI315" s="12">
-        <v>2</v>
-      </c>
-      <c r="AJ315" s="12">
-        <v>3</v>
-      </c>
-      <c r="AK315" s="12">
+      <c r="AE315">
+        <v>1</v>
+      </c>
+      <c r="AF315">
+        <v>1</v>
+      </c>
+      <c r="AG315">
+        <v>2</v>
+      </c>
+      <c r="AH315">
+        <v>2</v>
+      </c>
+      <c r="AI315">
+        <v>2</v>
+      </c>
+      <c r="AJ315">
+        <v>3</v>
+      </c>
+      <c r="AK315">
         <v>5</v>
       </c>
-      <c r="AL315" s="12">
-        <v>1</v>
-      </c>
-      <c r="AM315" s="12">
-        <v>2</v>
-      </c>
-      <c r="AN315" s="12">
-        <v>2</v>
-      </c>
-      <c r="AO315" s="12">
-        <v>0</v>
-      </c>
-      <c r="AP315" s="12">
-        <v>0</v>
-      </c>
-      <c r="AQ315" s="12">
-        <v>0</v>
-      </c>
-      <c r="AR315" s="12">
-        <v>0</v>
-      </c>
-      <c r="AS315" s="12">
-        <v>0</v>
-      </c>
-      <c r="AT315" s="12">
+      <c r="AL315">
+        <v>1</v>
+      </c>
+      <c r="AM315">
+        <v>2</v>
+      </c>
+      <c r="AN315">
+        <v>2</v>
+      </c>
+      <c r="AO315">
+        <v>0</v>
+      </c>
+      <c r="AP315">
+        <v>0</v>
+      </c>
+      <c r="AQ315">
+        <v>0</v>
+      </c>
+      <c r="AR315">
+        <v>0</v>
+      </c>
+      <c r="AS315">
+        <v>0</v>
+      </c>
+      <c r="AT315">
         <v>0</v>
       </c>
     </row>
     <row r="316" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A316" s="12" t="s">
+      <c r="A316" t="s">
         <v>264</v>
       </c>
-      <c r="B316" s="13" t="s">
+      <c r="B316" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="C316" s="14">
+      <c r="C316" s="4">
         <v>7.4</v>
       </c>
-      <c r="D316" s="12">
+      <c r="D316">
         <v>64</v>
       </c>
-      <c r="E316" s="12">
-        <v>0</v>
-      </c>
-      <c r="F316" s="12">
-        <v>2</v>
-      </c>
-      <c r="G316" s="12">
-        <v>0</v>
-      </c>
-      <c r="H316" s="12">
-        <v>0</v>
-      </c>
-      <c r="I316" s="12">
-        <v>0</v>
-      </c>
-      <c r="J316" s="12">
-        <v>0</v>
-      </c>
-      <c r="K316" s="12">
-        <v>0</v>
-      </c>
-      <c r="L316" s="12">
-        <v>0</v>
-      </c>
-      <c r="M316" s="12">
-        <v>0</v>
-      </c>
-      <c r="N316" s="12">
+      <c r="E316">
+        <v>0</v>
+      </c>
+      <c r="F316">
+        <v>2</v>
+      </c>
+      <c r="G316">
+        <v>0</v>
+      </c>
+      <c r="H316">
+        <v>0</v>
+      </c>
+      <c r="I316">
+        <v>0</v>
+      </c>
+      <c r="J316">
+        <v>0</v>
+      </c>
+      <c r="K316">
+        <v>0</v>
+      </c>
+      <c r="L316">
+        <v>0</v>
+      </c>
+      <c r="M316">
+        <v>0</v>
+      </c>
+      <c r="N316">
         <v>5</v>
       </c>
-      <c r="O316" s="12">
-        <v>0</v>
-      </c>
-      <c r="P316" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q316" s="12">
+      <c r="O316">
+        <v>0</v>
+      </c>
+      <c r="P316">
+        <v>0</v>
+      </c>
+      <c r="Q316">
         <v>34</v>
       </c>
-      <c r="R316" s="12">
+      <c r="R316">
         <v>38</v>
       </c>
-      <c r="S316" s="12">
+      <c r="S316">
         <v>28</v>
       </c>
-      <c r="T316" s="12">
+      <c r="T316">
         <v>32</v>
       </c>
-      <c r="U316" s="12">
+      <c r="U316">
         <v>6</v>
       </c>
-      <c r="V316" s="12">
+      <c r="V316">
         <v>6</v>
       </c>
-      <c r="W316" s="12">
-        <v>2</v>
-      </c>
-      <c r="X316" s="12">
-        <v>3</v>
-      </c>
-      <c r="Y316" s="12">
+      <c r="W316">
+        <v>2</v>
+      </c>
+      <c r="X316">
+        <v>3</v>
+      </c>
+      <c r="Y316">
         <v>47</v>
       </c>
-      <c r="Z316" s="12">
-        <v>1</v>
-      </c>
-      <c r="AA316" s="12">
-        <v>2</v>
-      </c>
-      <c r="AB316" s="12">
-        <v>3</v>
-      </c>
-      <c r="AC316" s="12">
-        <v>0</v>
-      </c>
-      <c r="AD316" s="12">
+      <c r="Z316">
+        <v>1</v>
+      </c>
+      <c r="AA316">
+        <v>2</v>
+      </c>
+      <c r="AB316">
+        <v>3</v>
+      </c>
+      <c r="AC316">
+        <v>0</v>
+      </c>
+      <c r="AD316">
         <v>7</v>
       </c>
-      <c r="AE316" s="12">
-        <v>0</v>
-      </c>
-      <c r="AF316" s="12">
-        <v>0</v>
-      </c>
-      <c r="AG316" s="12">
-        <v>0</v>
-      </c>
-      <c r="AH316" s="12">
-        <v>0</v>
-      </c>
-      <c r="AI316" s="12">
-        <v>1</v>
-      </c>
-      <c r="AJ316" s="12">
-        <v>2</v>
-      </c>
-      <c r="AK316" s="12">
+      <c r="AE316">
+        <v>0</v>
+      </c>
+      <c r="AF316">
+        <v>0</v>
+      </c>
+      <c r="AG316">
+        <v>0</v>
+      </c>
+      <c r="AH316">
+        <v>0</v>
+      </c>
+      <c r="AI316">
+        <v>1</v>
+      </c>
+      <c r="AJ316">
+        <v>2</v>
+      </c>
+      <c r="AK316">
         <v>4</v>
       </c>
-      <c r="AL316" s="12">
-        <v>0</v>
-      </c>
-      <c r="AM316" s="12">
-        <v>0</v>
-      </c>
-      <c r="AN316" s="12">
-        <v>0</v>
-      </c>
-      <c r="AO316" s="12">
-        <v>0</v>
-      </c>
-      <c r="AP316" s="12">
-        <v>0</v>
-      </c>
-      <c r="AQ316" s="12">
-        <v>0</v>
-      </c>
-      <c r="AR316" s="12">
-        <v>0</v>
-      </c>
-      <c r="AS316" s="12">
-        <v>0</v>
-      </c>
-      <c r="AT316" s="12">
+      <c r="AL316">
+        <v>0</v>
+      </c>
+      <c r="AM316">
+        <v>0</v>
+      </c>
+      <c r="AN316">
+        <v>0</v>
+      </c>
+      <c r="AO316">
+        <v>0</v>
+      </c>
+      <c r="AP316">
+        <v>0</v>
+      </c>
+      <c r="AQ316">
+        <v>0</v>
+      </c>
+      <c r="AR316">
+        <v>0</v>
+      </c>
+      <c r="AS316">
+        <v>0</v>
+      </c>
+      <c r="AT316">
         <v>0</v>
       </c>
     </row>
     <row r="317" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A317" s="12" t="s">
+      <c r="A317" t="s">
         <v>264</v>
       </c>
-      <c r="B317" s="13" t="s">
+      <c r="B317" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C317" s="14">
+      <c r="C317" s="4">
         <v>7.7</v>
       </c>
-      <c r="D317" s="12">
+      <c r="D317">
         <v>65</v>
       </c>
-      <c r="E317" s="12">
-        <v>0</v>
-      </c>
-      <c r="F317" s="12">
-        <v>2</v>
-      </c>
-      <c r="G317" s="12">
-        <v>2</v>
-      </c>
-      <c r="H317" s="12">
-        <v>0</v>
-      </c>
-      <c r="I317" s="12">
-        <v>0</v>
-      </c>
-      <c r="J317" s="12">
-        <v>0</v>
-      </c>
-      <c r="K317" s="12">
-        <v>1</v>
-      </c>
-      <c r="L317" s="12">
-        <v>0</v>
-      </c>
-      <c r="M317" s="12">
-        <v>0</v>
-      </c>
-      <c r="N317" s="12">
-        <v>3</v>
-      </c>
-      <c r="O317" s="12">
-        <v>1</v>
-      </c>
-      <c r="P317" s="12">
+      <c r="E317">
+        <v>0</v>
+      </c>
+      <c r="F317">
+        <v>2</v>
+      </c>
+      <c r="G317">
+        <v>2</v>
+      </c>
+      <c r="H317">
+        <v>0</v>
+      </c>
+      <c r="I317">
+        <v>0</v>
+      </c>
+      <c r="J317">
+        <v>0</v>
+      </c>
+      <c r="K317">
+        <v>1</v>
+      </c>
+      <c r="L317">
+        <v>0</v>
+      </c>
+      <c r="M317">
+        <v>0</v>
+      </c>
+      <c r="N317">
+        <v>3</v>
+      </c>
+      <c r="O317">
+        <v>1</v>
+      </c>
+      <c r="P317">
         <v>7</v>
       </c>
-      <c r="Q317" s="12">
+      <c r="Q317">
         <v>55</v>
       </c>
-      <c r="R317" s="12">
+      <c r="R317">
         <v>58</v>
       </c>
-      <c r="S317" s="12">
+      <c r="S317">
         <v>34</v>
       </c>
-      <c r="T317" s="12">
+      <c r="T317">
         <v>41</v>
       </c>
-      <c r="U317" s="12">
+      <c r="U317">
         <v>16</v>
       </c>
-      <c r="V317" s="12">
+      <c r="V317">
         <v>17</v>
       </c>
-      <c r="W317" s="12">
-        <v>3</v>
-      </c>
-      <c r="X317" s="12">
+      <c r="W317">
+        <v>3</v>
+      </c>
+      <c r="X317">
         <v>4</v>
       </c>
-      <c r="Y317" s="12">
+      <c r="Y317">
         <v>75</v>
       </c>
-      <c r="Z317" s="12">
-        <v>0</v>
-      </c>
-      <c r="AA317" s="12">
-        <v>1</v>
-      </c>
-      <c r="AB317" s="12">
-        <v>2</v>
-      </c>
-      <c r="AC317" s="12">
-        <v>2</v>
-      </c>
-      <c r="AD317" s="12">
+      <c r="Z317">
+        <v>0</v>
+      </c>
+      <c r="AA317">
+        <v>1</v>
+      </c>
+      <c r="AB317">
+        <v>2</v>
+      </c>
+      <c r="AC317">
+        <v>2</v>
+      </c>
+      <c r="AD317">
         <v>13</v>
       </c>
-      <c r="AE317" s="12">
-        <v>0</v>
-      </c>
-      <c r="AF317" s="12">
-        <v>0</v>
-      </c>
-      <c r="AG317" s="12">
-        <v>0</v>
-      </c>
-      <c r="AH317" s="12">
-        <v>0</v>
-      </c>
-      <c r="AI317" s="12">
-        <v>0</v>
-      </c>
-      <c r="AJ317" s="12">
-        <v>3</v>
-      </c>
-      <c r="AK317" s="12">
+      <c r="AE317">
+        <v>0</v>
+      </c>
+      <c r="AF317">
+        <v>0</v>
+      </c>
+      <c r="AG317">
+        <v>0</v>
+      </c>
+      <c r="AH317">
+        <v>0</v>
+      </c>
+      <c r="AI317">
+        <v>0</v>
+      </c>
+      <c r="AJ317">
+        <v>3</v>
+      </c>
+      <c r="AK317">
         <v>5</v>
       </c>
-      <c r="AL317" s="12">
-        <v>0</v>
-      </c>
-      <c r="AM317" s="12">
-        <v>0</v>
-      </c>
-      <c r="AN317" s="12">
-        <v>0</v>
-      </c>
-      <c r="AO317" s="12">
-        <v>0</v>
-      </c>
-      <c r="AP317" s="12">
-        <v>0</v>
-      </c>
-      <c r="AQ317" s="12">
-        <v>0</v>
-      </c>
-      <c r="AR317" s="12">
-        <v>0</v>
-      </c>
-      <c r="AS317" s="12">
-        <v>0</v>
-      </c>
-      <c r="AT317" s="12">
+      <c r="AL317">
+        <v>0</v>
+      </c>
+      <c r="AM317">
+        <v>0</v>
+      </c>
+      <c r="AN317">
+        <v>0</v>
+      </c>
+      <c r="AO317">
+        <v>0</v>
+      </c>
+      <c r="AP317">
+        <v>0</v>
+      </c>
+      <c r="AQ317">
+        <v>0</v>
+      </c>
+      <c r="AR317">
+        <v>0</v>
+      </c>
+      <c r="AS317">
+        <v>0</v>
+      </c>
+      <c r="AT317">
         <v>0</v>
       </c>
     </row>
     <row r="318" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A318" s="12" t="s">
+      <c r="A318" t="s">
         <v>264</v>
       </c>
-      <c r="B318" s="13" t="s">
+      <c r="B318" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C318" s="14">
+      <c r="C318" s="4">
         <v>7</v>
       </c>
-      <c r="D318" s="12">
+      <c r="D318">
         <v>77</v>
       </c>
-      <c r="E318" s="12">
-        <v>0</v>
-      </c>
-      <c r="F318" s="12">
-        <v>3</v>
-      </c>
-      <c r="G318" s="12">
-        <v>1</v>
-      </c>
-      <c r="H318" s="12">
-        <v>0</v>
-      </c>
-      <c r="I318" s="12">
-        <v>0</v>
-      </c>
-      <c r="J318" s="12">
-        <v>0</v>
-      </c>
-      <c r="K318" s="12">
-        <v>0</v>
-      </c>
-      <c r="L318" s="12">
-        <v>0</v>
-      </c>
-      <c r="M318" s="12">
-        <v>0</v>
-      </c>
-      <c r="N318" s="12">
-        <v>2</v>
-      </c>
-      <c r="O318" s="12">
-        <v>1</v>
-      </c>
-      <c r="P318" s="12">
-        <v>2</v>
-      </c>
-      <c r="Q318" s="12">
+      <c r="E318">
+        <v>0</v>
+      </c>
+      <c r="F318">
+        <v>3</v>
+      </c>
+      <c r="G318">
+        <v>1</v>
+      </c>
+      <c r="H318">
+        <v>0</v>
+      </c>
+      <c r="I318">
+        <v>0</v>
+      </c>
+      <c r="J318">
+        <v>0</v>
+      </c>
+      <c r="K318">
+        <v>0</v>
+      </c>
+      <c r="L318">
+        <v>0</v>
+      </c>
+      <c r="M318">
+        <v>0</v>
+      </c>
+      <c r="N318">
+        <v>2</v>
+      </c>
+      <c r="O318">
+        <v>1</v>
+      </c>
+      <c r="P318">
+        <v>2</v>
+      </c>
+      <c r="Q318">
         <v>50</v>
       </c>
-      <c r="R318" s="12">
+      <c r="R318">
         <v>51</v>
       </c>
-      <c r="S318" s="12">
+      <c r="S318">
         <v>27</v>
       </c>
-      <c r="T318" s="12">
+      <c r="T318">
         <v>28</v>
       </c>
-      <c r="U318" s="12">
+      <c r="U318">
         <v>22</v>
       </c>
-      <c r="V318" s="12">
+      <c r="V318">
         <v>23</v>
       </c>
-      <c r="W318" s="12">
-        <v>0</v>
-      </c>
-      <c r="X318" s="12">
-        <v>0</v>
-      </c>
-      <c r="Y318" s="12">
+      <c r="W318">
+        <v>0</v>
+      </c>
+      <c r="X318">
+        <v>0</v>
+      </c>
+      <c r="Y318">
         <v>67</v>
       </c>
-      <c r="Z318" s="12">
-        <v>2</v>
-      </c>
-      <c r="AA318" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB318" s="12">
-        <v>1</v>
-      </c>
-      <c r="AC318" s="12">
-        <v>2</v>
-      </c>
-      <c r="AD318" s="12">
+      <c r="Z318">
+        <v>2</v>
+      </c>
+      <c r="AA318">
+        <v>0</v>
+      </c>
+      <c r="AB318">
+        <v>1</v>
+      </c>
+      <c r="AC318">
+        <v>2</v>
+      </c>
+      <c r="AD318">
         <v>7</v>
       </c>
-      <c r="AE318" s="12">
-        <v>1</v>
-      </c>
-      <c r="AF318" s="12">
+      <c r="AE318">
+        <v>1</v>
+      </c>
+      <c r="AF318">
         <v>4</v>
       </c>
-      <c r="AG318" s="12">
-        <v>0</v>
-      </c>
-      <c r="AH318" s="12">
-        <v>0</v>
-      </c>
-      <c r="AI318" s="12">
-        <v>3</v>
-      </c>
-      <c r="AJ318" s="12">
+      <c r="AG318">
+        <v>0</v>
+      </c>
+      <c r="AH318">
+        <v>0</v>
+      </c>
+      <c r="AI318">
+        <v>3</v>
+      </c>
+      <c r="AJ318">
         <v>6</v>
       </c>
-      <c r="AK318" s="12">
+      <c r="AK318">
         <v>12</v>
       </c>
-      <c r="AL318" s="12">
-        <v>0</v>
-      </c>
-      <c r="AM318" s="12">
-        <v>1</v>
-      </c>
-      <c r="AN318" s="12">
-        <v>2</v>
-      </c>
-      <c r="AO318" s="12">
-        <v>1</v>
-      </c>
-      <c r="AP318" s="12">
-        <v>0</v>
-      </c>
-      <c r="AQ318" s="12">
-        <v>0</v>
-      </c>
-      <c r="AR318" s="12">
-        <v>0</v>
-      </c>
-      <c r="AS318" s="12">
-        <v>0</v>
-      </c>
-      <c r="AT318" s="12">
+      <c r="AL318">
+        <v>0</v>
+      </c>
+      <c r="AM318">
+        <v>1</v>
+      </c>
+      <c r="AN318">
+        <v>2</v>
+      </c>
+      <c r="AO318">
+        <v>1</v>
+      </c>
+      <c r="AP318">
+        <v>0</v>
+      </c>
+      <c r="AQ318">
+        <v>0</v>
+      </c>
+      <c r="AR318">
+        <v>0</v>
+      </c>
+      <c r="AS318">
+        <v>0</v>
+      </c>
+      <c r="AT318">
         <v>0</v>
       </c>
     </row>
     <row r="319" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A319" s="12" t="s">
+      <c r="A319" t="s">
         <v>264</v>
       </c>
-      <c r="B319" s="13" t="s">
+      <c r="B319" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C319" s="14">
+      <c r="C319" s="4">
         <v>6.7</v>
       </c>
-      <c r="D319" s="12">
+      <c r="D319">
         <v>77</v>
       </c>
-      <c r="E319" s="12">
-        <v>0</v>
-      </c>
-      <c r="F319" s="12">
-        <v>2</v>
-      </c>
-      <c r="G319" s="12">
-        <v>0</v>
-      </c>
-      <c r="H319" s="12">
-        <v>0</v>
-      </c>
-      <c r="I319" s="12">
-        <v>0</v>
-      </c>
-      <c r="J319" s="12">
-        <v>0</v>
-      </c>
-      <c r="K319" s="12">
-        <v>1</v>
-      </c>
-      <c r="L319" s="12">
-        <v>0</v>
-      </c>
-      <c r="M319" s="12">
-        <v>0</v>
-      </c>
-      <c r="N319" s="12">
-        <v>1</v>
-      </c>
-      <c r="O319" s="12">
-        <v>0</v>
-      </c>
-      <c r="P319" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q319" s="12">
+      <c r="E319">
+        <v>0</v>
+      </c>
+      <c r="F319">
+        <v>2</v>
+      </c>
+      <c r="G319">
+        <v>0</v>
+      </c>
+      <c r="H319">
+        <v>0</v>
+      </c>
+      <c r="I319">
+        <v>0</v>
+      </c>
+      <c r="J319">
+        <v>0</v>
+      </c>
+      <c r="K319">
+        <v>1</v>
+      </c>
+      <c r="L319">
+        <v>0</v>
+      </c>
+      <c r="M319">
+        <v>0</v>
+      </c>
+      <c r="N319">
+        <v>1</v>
+      </c>
+      <c r="O319">
+        <v>0</v>
+      </c>
+      <c r="P319">
+        <v>0</v>
+      </c>
+      <c r="Q319">
         <v>12</v>
       </c>
-      <c r="R319" s="12">
+      <c r="R319">
         <v>13</v>
       </c>
-      <c r="S319" s="12">
+      <c r="S319">
         <v>9</v>
       </c>
-      <c r="T319" s="12">
+      <c r="T319">
         <v>10</v>
       </c>
-      <c r="U319" s="12">
-        <v>3</v>
-      </c>
-      <c r="V319" s="12">
-        <v>3</v>
-      </c>
-      <c r="W319" s="12">
-        <v>0</v>
-      </c>
-      <c r="X319" s="12">
-        <v>0</v>
-      </c>
-      <c r="Y319" s="12">
+      <c r="U319">
+        <v>3</v>
+      </c>
+      <c r="V319">
+        <v>3</v>
+      </c>
+      <c r="W319">
+        <v>0</v>
+      </c>
+      <c r="X319">
+        <v>0</v>
+      </c>
+      <c r="Y319">
         <v>21</v>
       </c>
-      <c r="Z319" s="12">
-        <v>1</v>
-      </c>
-      <c r="AA319" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB319" s="12">
-        <v>0</v>
-      </c>
-      <c r="AC319" s="12">
-        <v>0</v>
-      </c>
-      <c r="AD319" s="12">
+      <c r="Z319">
+        <v>1</v>
+      </c>
+      <c r="AA319">
+        <v>0</v>
+      </c>
+      <c r="AB319">
+        <v>0</v>
+      </c>
+      <c r="AC319">
+        <v>0</v>
+      </c>
+      <c r="AD319">
         <v>5</v>
       </c>
-      <c r="AE319" s="12">
-        <v>0</v>
-      </c>
-      <c r="AF319" s="12">
-        <v>0</v>
-      </c>
-      <c r="AG319" s="12">
-        <v>0</v>
-      </c>
-      <c r="AH319" s="12">
-        <v>1</v>
-      </c>
-      <c r="AI319" s="12">
-        <v>3</v>
-      </c>
-      <c r="AJ319" s="12">
-        <v>0</v>
-      </c>
-      <c r="AK319" s="12">
+      <c r="AE319">
+        <v>0</v>
+      </c>
+      <c r="AF319">
+        <v>0</v>
+      </c>
+      <c r="AG319">
+        <v>0</v>
+      </c>
+      <c r="AH319">
+        <v>1</v>
+      </c>
+      <c r="AI319">
+        <v>3</v>
+      </c>
+      <c r="AJ319">
+        <v>0</v>
+      </c>
+      <c r="AK319">
         <v>5</v>
       </c>
-      <c r="AL319" s="12">
-        <v>0</v>
-      </c>
-      <c r="AM319" s="12">
-        <v>0</v>
-      </c>
-      <c r="AN319" s="12">
-        <v>2</v>
-      </c>
-      <c r="AO319" s="12">
-        <v>0</v>
-      </c>
-      <c r="AP319" s="12">
-        <v>0</v>
-      </c>
-      <c r="AQ319" s="12">
-        <v>0</v>
-      </c>
-      <c r="AR319" s="12">
-        <v>0</v>
-      </c>
-      <c r="AS319" s="12">
-        <v>0</v>
-      </c>
-      <c r="AT319" s="12">
+      <c r="AL319">
+        <v>0</v>
+      </c>
+      <c r="AM319">
+        <v>0</v>
+      </c>
+      <c r="AN319">
+        <v>2</v>
+      </c>
+      <c r="AO319">
+        <v>0</v>
+      </c>
+      <c r="AP319">
+        <v>0</v>
+      </c>
+      <c r="AQ319">
+        <v>0</v>
+      </c>
+      <c r="AR319">
+        <v>0</v>
+      </c>
+      <c r="AS319">
+        <v>0</v>
+      </c>
+      <c r="AT319">
         <v>0</v>
       </c>
     </row>
     <row r="320" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A320" s="12" t="s">
+      <c r="A320" t="s">
         <v>264</v>
       </c>
-      <c r="B320" s="13" t="s">
+      <c r="B320" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C320" s="14">
+      <c r="C320" s="4">
         <v>6.5</v>
       </c>
-      <c r="D320" s="12">
+      <c r="D320">
         <v>45</v>
       </c>
-      <c r="E320" s="12">
-        <v>0</v>
-      </c>
-      <c r="F320" s="12">
-        <v>0</v>
-      </c>
-      <c r="G320" s="12">
-        <v>0</v>
-      </c>
-      <c r="H320" s="12">
-        <v>0</v>
-      </c>
-      <c r="I320" s="12">
-        <v>0</v>
-      </c>
-      <c r="J320" s="12">
-        <v>0</v>
-      </c>
-      <c r="K320" s="12">
-        <v>0</v>
-      </c>
-      <c r="L320" s="12">
-        <v>0</v>
-      </c>
-      <c r="M320" s="12">
-        <v>0</v>
-      </c>
-      <c r="N320" s="12">
-        <v>0</v>
-      </c>
-      <c r="O320" s="12">
-        <v>0</v>
-      </c>
-      <c r="P320" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q320" s="12">
+      <c r="E320">
+        <v>0</v>
+      </c>
+      <c r="F320">
+        <v>0</v>
+      </c>
+      <c r="G320">
+        <v>0</v>
+      </c>
+      <c r="H320">
+        <v>0</v>
+      </c>
+      <c r="I320">
+        <v>0</v>
+      </c>
+      <c r="J320">
+        <v>0</v>
+      </c>
+      <c r="K320">
+        <v>0</v>
+      </c>
+      <c r="L320">
+        <v>0</v>
+      </c>
+      <c r="M320">
+        <v>0</v>
+      </c>
+      <c r="N320">
+        <v>0</v>
+      </c>
+      <c r="O320">
+        <v>0</v>
+      </c>
+      <c r="P320">
+        <v>0</v>
+      </c>
+      <c r="Q320">
         <v>23</v>
       </c>
-      <c r="R320" s="12">
+      <c r="R320">
         <v>24</v>
       </c>
-      <c r="S320" s="12">
+      <c r="S320">
         <v>8</v>
       </c>
-      <c r="T320" s="12">
+      <c r="T320">
         <v>9</v>
       </c>
-      <c r="U320" s="12">
+      <c r="U320">
         <v>15</v>
       </c>
-      <c r="V320" s="12">
+      <c r="V320">
         <v>15</v>
       </c>
-      <c r="W320" s="12">
-        <v>2</v>
-      </c>
-      <c r="X320" s="12">
-        <v>3</v>
-      </c>
-      <c r="Y320" s="12">
+      <c r="W320">
+        <v>2</v>
+      </c>
+      <c r="X320">
+        <v>3</v>
+      </c>
+      <c r="Y320">
         <v>26</v>
       </c>
-      <c r="Z320" s="12">
-        <v>1</v>
-      </c>
-      <c r="AA320" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB320" s="12">
-        <v>0</v>
-      </c>
-      <c r="AC320" s="12">
-        <v>0</v>
-      </c>
-      <c r="AD320" s="12">
-        <v>2</v>
-      </c>
-      <c r="AE320" s="12">
-        <v>0</v>
-      </c>
-      <c r="AF320" s="12">
-        <v>0</v>
-      </c>
-      <c r="AG320" s="12">
-        <v>0</v>
-      </c>
-      <c r="AH320" s="12">
-        <v>1</v>
-      </c>
-      <c r="AI320" s="12">
-        <v>2</v>
-      </c>
-      <c r="AJ320" s="12">
-        <v>0</v>
-      </c>
-      <c r="AK320" s="12">
-        <v>0</v>
-      </c>
-      <c r="AL320" s="12">
-        <v>0</v>
-      </c>
-      <c r="AM320" s="12">
-        <v>0</v>
-      </c>
-      <c r="AN320" s="12">
-        <v>0</v>
-      </c>
-      <c r="AO320" s="12">
-        <v>0</v>
-      </c>
-      <c r="AP320" s="12">
-        <v>0</v>
-      </c>
-      <c r="AQ320" s="12">
-        <v>0</v>
-      </c>
-      <c r="AR320" s="12">
-        <v>0</v>
-      </c>
-      <c r="AS320" s="12">
-        <v>0</v>
-      </c>
-      <c r="AT320" s="12">
+      <c r="Z320">
+        <v>1</v>
+      </c>
+      <c r="AA320">
+        <v>0</v>
+      </c>
+      <c r="AB320">
+        <v>0</v>
+      </c>
+      <c r="AC320">
+        <v>0</v>
+      </c>
+      <c r="AD320">
+        <v>2</v>
+      </c>
+      <c r="AE320">
+        <v>0</v>
+      </c>
+      <c r="AF320">
+        <v>0</v>
+      </c>
+      <c r="AG320">
+        <v>0</v>
+      </c>
+      <c r="AH320">
+        <v>1</v>
+      </c>
+      <c r="AI320">
+        <v>2</v>
+      </c>
+      <c r="AJ320">
+        <v>0</v>
+      </c>
+      <c r="AK320">
+        <v>0</v>
+      </c>
+      <c r="AL320">
+        <v>0</v>
+      </c>
+      <c r="AM320">
+        <v>0</v>
+      </c>
+      <c r="AN320">
+        <v>0</v>
+      </c>
+      <c r="AO320">
+        <v>0</v>
+      </c>
+      <c r="AP320">
+        <v>0</v>
+      </c>
+      <c r="AQ320">
+        <v>0</v>
+      </c>
+      <c r="AR320">
+        <v>0</v>
+      </c>
+      <c r="AS320">
+        <v>0</v>
+      </c>
+      <c r="AT320">
         <v>0</v>
       </c>
     </row>
     <row r="321" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A321" s="12" t="s">
+      <c r="A321" t="s">
         <v>264</v>
       </c>
-      <c r="B321" s="13" t="s">
+      <c r="B321" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C321" s="14">
+      <c r="C321" s="4">
         <v>6.5</v>
       </c>
-      <c r="D321" s="12">
+      <c r="D321">
         <v>26</v>
       </c>
-      <c r="E321" s="12">
-        <v>0</v>
-      </c>
-      <c r="F321" s="12">
-        <v>0</v>
-      </c>
-      <c r="G321" s="12">
-        <v>0</v>
-      </c>
-      <c r="H321" s="12">
-        <v>0</v>
-      </c>
-      <c r="I321" s="12">
-        <v>0</v>
-      </c>
-      <c r="J321" s="12">
-        <v>0</v>
-      </c>
-      <c r="K321" s="12">
-        <v>0</v>
-      </c>
-      <c r="L321" s="12">
-        <v>0</v>
-      </c>
-      <c r="M321" s="12">
-        <v>0</v>
-      </c>
-      <c r="N321" s="12">
-        <v>0</v>
-      </c>
-      <c r="O321" s="12">
-        <v>0</v>
-      </c>
-      <c r="P321" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q321" s="12">
+      <c r="E321">
+        <v>0</v>
+      </c>
+      <c r="F321">
+        <v>0</v>
+      </c>
+      <c r="G321">
+        <v>0</v>
+      </c>
+      <c r="H321">
+        <v>0</v>
+      </c>
+      <c r="I321">
+        <v>0</v>
+      </c>
+      <c r="J321">
+        <v>0</v>
+      </c>
+      <c r="K321">
+        <v>0</v>
+      </c>
+      <c r="L321">
+        <v>0</v>
+      </c>
+      <c r="M321">
+        <v>0</v>
+      </c>
+      <c r="N321">
+        <v>0</v>
+      </c>
+      <c r="O321">
+        <v>0</v>
+      </c>
+      <c r="P321">
+        <v>0</v>
+      </c>
+      <c r="Q321">
         <v>11</v>
       </c>
-      <c r="R321" s="12">
+      <c r="R321">
         <v>12</v>
       </c>
-      <c r="S321" s="12">
-        <v>3</v>
-      </c>
-      <c r="T321" s="12">
-        <v>3</v>
-      </c>
-      <c r="U321" s="12">
+      <c r="S321">
+        <v>3</v>
+      </c>
+      <c r="T321">
+        <v>3</v>
+      </c>
+      <c r="U321">
         <v>8</v>
       </c>
-      <c r="V321" s="12">
+      <c r="V321">
         <v>9</v>
       </c>
-      <c r="W321" s="12">
-        <v>1</v>
-      </c>
-      <c r="X321" s="12">
-        <v>1</v>
-      </c>
-      <c r="Y321" s="12">
+      <c r="W321">
+        <v>1</v>
+      </c>
+      <c r="X321">
+        <v>1</v>
+      </c>
+      <c r="Y321">
         <v>14</v>
       </c>
-      <c r="Z321" s="12">
-        <v>0</v>
-      </c>
-      <c r="AA321" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB321" s="12">
-        <v>0</v>
-      </c>
-      <c r="AC321" s="12">
-        <v>0</v>
-      </c>
-      <c r="AD321" s="12">
-        <v>1</v>
-      </c>
-      <c r="AE321" s="12">
-        <v>1</v>
-      </c>
-      <c r="AF321" s="12">
-        <v>1</v>
-      </c>
-      <c r="AG321" s="12">
-        <v>0</v>
-      </c>
-      <c r="AH321" s="12">
-        <v>0</v>
-      </c>
-      <c r="AI321" s="12">
-        <v>1</v>
-      </c>
-      <c r="AJ321" s="12">
-        <v>1</v>
-      </c>
-      <c r="AK321" s="12">
+      <c r="Z321">
+        <v>0</v>
+      </c>
+      <c r="AA321">
+        <v>0</v>
+      </c>
+      <c r="AB321">
+        <v>0</v>
+      </c>
+      <c r="AC321">
+        <v>0</v>
+      </c>
+      <c r="AD321">
+        <v>1</v>
+      </c>
+      <c r="AE321">
+        <v>1</v>
+      </c>
+      <c r="AF321">
+        <v>1</v>
+      </c>
+      <c r="AG321">
+        <v>0</v>
+      </c>
+      <c r="AH321">
+        <v>0</v>
+      </c>
+      <c r="AI321">
+        <v>1</v>
+      </c>
+      <c r="AJ321">
+        <v>1</v>
+      </c>
+      <c r="AK321">
         <v>4</v>
       </c>
-      <c r="AL321" s="12">
-        <v>0</v>
-      </c>
-      <c r="AM321" s="12">
-        <v>0</v>
-      </c>
-      <c r="AN321" s="12">
-        <v>3</v>
-      </c>
-      <c r="AO321" s="12">
-        <v>0</v>
-      </c>
-      <c r="AP321" s="12">
-        <v>0</v>
-      </c>
-      <c r="AQ321" s="12">
-        <v>0</v>
-      </c>
-      <c r="AR321" s="12">
-        <v>0</v>
-      </c>
-      <c r="AS321" s="12">
-        <v>0</v>
-      </c>
-      <c r="AT321" s="12">
+      <c r="AL321">
+        <v>0</v>
+      </c>
+      <c r="AM321">
+        <v>0</v>
+      </c>
+      <c r="AN321">
+        <v>3</v>
+      </c>
+      <c r="AO321">
+        <v>0</v>
+      </c>
+      <c r="AP321">
+        <v>0</v>
+      </c>
+      <c r="AQ321">
+        <v>0</v>
+      </c>
+      <c r="AR321">
+        <v>0</v>
+      </c>
+      <c r="AS321">
+        <v>0</v>
+      </c>
+      <c r="AT321">
         <v>0</v>
       </c>
     </row>
     <row r="322" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A322" s="12" t="s">
+      <c r="A322" t="s">
         <v>264</v>
       </c>
-      <c r="B322" s="13" t="s">
+      <c r="B322" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C322" s="14">
+      <c r="C322" s="4">
         <v>6.9</v>
       </c>
-      <c r="D322" s="12">
+      <c r="D322">
         <v>26</v>
       </c>
-      <c r="E322" s="12">
-        <v>0</v>
-      </c>
-      <c r="F322" s="12">
-        <v>2</v>
-      </c>
-      <c r="G322" s="12">
-        <v>0</v>
-      </c>
-      <c r="H322" s="12">
-        <v>0</v>
-      </c>
-      <c r="I322" s="12">
-        <v>0</v>
-      </c>
-      <c r="J322" s="12">
-        <v>0</v>
-      </c>
-      <c r="K322" s="12">
-        <v>0</v>
-      </c>
-      <c r="L322" s="12">
-        <v>0</v>
-      </c>
-      <c r="M322" s="12">
-        <v>0</v>
-      </c>
-      <c r="N322" s="12">
-        <v>2</v>
-      </c>
-      <c r="O322" s="12">
-        <v>1</v>
-      </c>
-      <c r="P322" s="12">
-        <v>2</v>
-      </c>
-      <c r="Q322" s="12">
+      <c r="E322">
+        <v>0</v>
+      </c>
+      <c r="F322">
+        <v>2</v>
+      </c>
+      <c r="G322">
+        <v>0</v>
+      </c>
+      <c r="H322">
+        <v>0</v>
+      </c>
+      <c r="I322">
+        <v>0</v>
+      </c>
+      <c r="J322">
+        <v>0</v>
+      </c>
+      <c r="K322">
+        <v>0</v>
+      </c>
+      <c r="L322">
+        <v>0</v>
+      </c>
+      <c r="M322">
+        <v>0</v>
+      </c>
+      <c r="N322">
+        <v>2</v>
+      </c>
+      <c r="O322">
+        <v>1</v>
+      </c>
+      <c r="P322">
+        <v>2</v>
+      </c>
+      <c r="Q322">
         <v>9</v>
       </c>
-      <c r="R322" s="12">
+      <c r="R322">
         <v>10</v>
       </c>
-      <c r="S322" s="12">
+      <c r="S322">
         <v>4</v>
       </c>
-      <c r="T322" s="12">
+      <c r="T322">
         <v>5</v>
       </c>
-      <c r="U322" s="12">
+      <c r="U322">
         <v>4</v>
       </c>
-      <c r="V322" s="12">
+      <c r="V322">
         <v>5</v>
       </c>
-      <c r="W322" s="12">
-        <v>0</v>
-      </c>
-      <c r="X322" s="12">
-        <v>0</v>
-      </c>
-      <c r="Y322" s="12">
+      <c r="W322">
+        <v>0</v>
+      </c>
+      <c r="X322">
+        <v>0</v>
+      </c>
+      <c r="Y322">
         <v>17</v>
       </c>
-      <c r="Z322" s="12">
-        <v>0</v>
-      </c>
-      <c r="AA322" s="12">
-        <v>2</v>
-      </c>
-      <c r="AB322" s="12">
-        <v>2</v>
-      </c>
-      <c r="AC322" s="12">
-        <v>1</v>
-      </c>
-      <c r="AD322" s="12">
-        <v>2</v>
-      </c>
-      <c r="AE322" s="12">
-        <v>0</v>
-      </c>
-      <c r="AF322" s="12">
-        <v>0</v>
-      </c>
-      <c r="AG322" s="12">
-        <v>0</v>
-      </c>
-      <c r="AH322" s="12">
-        <v>0</v>
-      </c>
-      <c r="AI322" s="12">
-        <v>2</v>
-      </c>
-      <c r="AJ322" s="12">
-        <v>3</v>
-      </c>
-      <c r="AK322" s="12">
-        <v>3</v>
-      </c>
-      <c r="AL322" s="12">
-        <v>0</v>
-      </c>
-      <c r="AM322" s="12">
-        <v>0</v>
-      </c>
-      <c r="AN322" s="12">
-        <v>0</v>
-      </c>
-      <c r="AO322" s="12">
-        <v>0</v>
-      </c>
-      <c r="AP322" s="12">
-        <v>0</v>
-      </c>
-      <c r="AQ322" s="12">
-        <v>0</v>
-      </c>
-      <c r="AR322" s="12">
-        <v>0</v>
-      </c>
-      <c r="AS322" s="12">
-        <v>0</v>
-      </c>
-      <c r="AT322" s="12">
+      <c r="Z322">
+        <v>0</v>
+      </c>
+      <c r="AA322">
+        <v>2</v>
+      </c>
+      <c r="AB322">
+        <v>2</v>
+      </c>
+      <c r="AC322">
+        <v>1</v>
+      </c>
+      <c r="AD322">
+        <v>2</v>
+      </c>
+      <c r="AE322">
+        <v>0</v>
+      </c>
+      <c r="AF322">
+        <v>0</v>
+      </c>
+      <c r="AG322">
+        <v>0</v>
+      </c>
+      <c r="AH322">
+        <v>0</v>
+      </c>
+      <c r="AI322">
+        <v>2</v>
+      </c>
+      <c r="AJ322">
+        <v>3</v>
+      </c>
+      <c r="AK322">
+        <v>3</v>
+      </c>
+      <c r="AL322">
+        <v>0</v>
+      </c>
+      <c r="AM322">
+        <v>0</v>
+      </c>
+      <c r="AN322">
+        <v>0</v>
+      </c>
+      <c r="AO322">
+        <v>0</v>
+      </c>
+      <c r="AP322">
+        <v>0</v>
+      </c>
+      <c r="AQ322">
+        <v>0</v>
+      </c>
+      <c r="AR322">
+        <v>0</v>
+      </c>
+      <c r="AS322">
+        <v>0</v>
+      </c>
+      <c r="AT322">
         <v>0</v>
       </c>
     </row>
     <row r="323" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A323" s="12" t="s">
+      <c r="A323" t="s">
         <v>264</v>
       </c>
-      <c r="B323" s="13" t="s">
+      <c r="B323" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C323" s="14">
+      <c r="C323" s="4">
         <v>7</v>
       </c>
-      <c r="D323" s="12">
+      <c r="D323">
         <v>25</v>
       </c>
-      <c r="E323" s="12">
-        <v>0</v>
-      </c>
-      <c r="F323" s="12">
-        <v>2</v>
-      </c>
-      <c r="G323" s="12">
-        <v>1</v>
-      </c>
-      <c r="H323" s="12">
-        <v>0</v>
-      </c>
-      <c r="I323" s="12">
-        <v>0</v>
-      </c>
-      <c r="J323" s="12">
-        <v>0</v>
-      </c>
-      <c r="K323" s="12">
-        <v>0</v>
-      </c>
-      <c r="L323" s="12">
-        <v>0</v>
-      </c>
-      <c r="M323" s="12">
-        <v>0</v>
-      </c>
-      <c r="N323" s="12">
-        <v>1</v>
-      </c>
-      <c r="O323" s="12">
-        <v>0</v>
-      </c>
-      <c r="P323" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q323" s="12">
+      <c r="E323">
+        <v>0</v>
+      </c>
+      <c r="F323">
+        <v>2</v>
+      </c>
+      <c r="G323">
+        <v>1</v>
+      </c>
+      <c r="H323">
+        <v>0</v>
+      </c>
+      <c r="I323">
+        <v>0</v>
+      </c>
+      <c r="J323">
+        <v>0</v>
+      </c>
+      <c r="K323">
+        <v>0</v>
+      </c>
+      <c r="L323">
+        <v>0</v>
+      </c>
+      <c r="M323">
+        <v>0</v>
+      </c>
+      <c r="N323">
+        <v>1</v>
+      </c>
+      <c r="O323">
+        <v>0</v>
+      </c>
+      <c r="P323">
+        <v>0</v>
+      </c>
+      <c r="Q323">
         <v>9</v>
       </c>
-      <c r="R323" s="12">
+      <c r="R323">
         <v>9</v>
       </c>
-      <c r="S323" s="12">
+      <c r="S323">
         <v>6</v>
       </c>
-      <c r="T323" s="12">
+      <c r="T323">
         <v>6</v>
       </c>
-      <c r="U323" s="12">
-        <v>3</v>
-      </c>
-      <c r="V323" s="12">
-        <v>3</v>
-      </c>
-      <c r="W323" s="12">
-        <v>1</v>
-      </c>
-      <c r="X323" s="12">
-        <v>1</v>
-      </c>
-      <c r="Y323" s="12">
+      <c r="U323">
+        <v>3</v>
+      </c>
+      <c r="V323">
+        <v>3</v>
+      </c>
+      <c r="W323">
+        <v>1</v>
+      </c>
+      <c r="X323">
+        <v>1</v>
+      </c>
+      <c r="Y323">
         <v>14</v>
       </c>
-      <c r="Z323" s="12">
-        <v>1</v>
-      </c>
-      <c r="AA323" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB323" s="12">
-        <v>0</v>
-      </c>
-      <c r="AC323" s="12">
-        <v>0</v>
-      </c>
-      <c r="AD323" s="12">
-        <v>1</v>
-      </c>
-      <c r="AE323" s="12">
-        <v>1</v>
-      </c>
-      <c r="AF323" s="12">
-        <v>1</v>
-      </c>
-      <c r="AG323" s="12">
-        <v>0</v>
-      </c>
-      <c r="AH323" s="12">
-        <v>0</v>
-      </c>
-      <c r="AI323" s="12">
-        <v>2</v>
-      </c>
-      <c r="AJ323" s="12">
-        <v>1</v>
-      </c>
-      <c r="AK323" s="12">
-        <v>3</v>
-      </c>
-      <c r="AL323" s="12">
-        <v>0</v>
-      </c>
-      <c r="AM323" s="12">
-        <v>0</v>
-      </c>
-      <c r="AN323" s="12">
-        <v>2</v>
-      </c>
-      <c r="AO323" s="12">
-        <v>0</v>
-      </c>
-      <c r="AP323" s="12">
-        <v>0</v>
-      </c>
-      <c r="AQ323" s="12">
-        <v>0</v>
-      </c>
-      <c r="AR323" s="12">
-        <v>0</v>
-      </c>
-      <c r="AS323" s="12">
-        <v>0</v>
-      </c>
-      <c r="AT323" s="12">
+      <c r="Z323">
+        <v>1</v>
+      </c>
+      <c r="AA323">
+        <v>0</v>
+      </c>
+      <c r="AB323">
+        <v>0</v>
+      </c>
+      <c r="AC323">
+        <v>0</v>
+      </c>
+      <c r="AD323">
+        <v>1</v>
+      </c>
+      <c r="AE323">
+        <v>1</v>
+      </c>
+      <c r="AF323">
+        <v>1</v>
+      </c>
+      <c r="AG323">
+        <v>0</v>
+      </c>
+      <c r="AH323">
+        <v>0</v>
+      </c>
+      <c r="AI323">
+        <v>2</v>
+      </c>
+      <c r="AJ323">
+        <v>1</v>
+      </c>
+      <c r="AK323">
+        <v>3</v>
+      </c>
+      <c r="AL323">
+        <v>0</v>
+      </c>
+      <c r="AM323">
+        <v>0</v>
+      </c>
+      <c r="AN323">
+        <v>2</v>
+      </c>
+      <c r="AO323">
+        <v>0</v>
+      </c>
+      <c r="AP323">
+        <v>0</v>
+      </c>
+      <c r="AQ323">
+        <v>0</v>
+      </c>
+      <c r="AR323">
+        <v>0</v>
+      </c>
+      <c r="AS323">
+        <v>0</v>
+      </c>
+      <c r="AT323">
         <v>0</v>
       </c>
     </row>
     <row r="324" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A324" s="12" t="s">
+      <c r="A324" t="s">
         <v>264</v>
       </c>
-      <c r="B324" s="13" t="s">
+      <c r="B324" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="C324" s="14">
+      <c r="C324" s="4">
         <v>7.3</v>
       </c>
-      <c r="D324" s="12">
+      <c r="D324">
         <v>13</v>
       </c>
-      <c r="E324" s="12">
-        <v>1</v>
-      </c>
-      <c r="F324" s="12">
-        <v>2</v>
-      </c>
-      <c r="G324" s="12">
-        <v>1</v>
-      </c>
-      <c r="H324" s="12">
-        <v>0</v>
-      </c>
-      <c r="I324" s="12">
-        <v>0</v>
-      </c>
-      <c r="J324" s="12">
-        <v>0</v>
-      </c>
-      <c r="K324" s="12">
-        <v>0</v>
-      </c>
-      <c r="L324" s="12">
-        <v>0</v>
-      </c>
-      <c r="M324" s="12">
-        <v>0</v>
-      </c>
-      <c r="N324" s="12">
-        <v>0</v>
-      </c>
-      <c r="O324" s="12">
-        <v>0</v>
-      </c>
-      <c r="P324" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q324" s="12">
+      <c r="E324">
+        <v>1</v>
+      </c>
+      <c r="F324">
+        <v>2</v>
+      </c>
+      <c r="G324">
+        <v>1</v>
+      </c>
+      <c r="H324">
+        <v>0</v>
+      </c>
+      <c r="I324">
+        <v>0</v>
+      </c>
+      <c r="J324">
+        <v>0</v>
+      </c>
+      <c r="K324">
+        <v>0</v>
+      </c>
+      <c r="L324">
+        <v>0</v>
+      </c>
+      <c r="M324">
+        <v>0</v>
+      </c>
+      <c r="N324">
+        <v>0</v>
+      </c>
+      <c r="O324">
+        <v>0</v>
+      </c>
+      <c r="P324">
+        <v>0</v>
+      </c>
+      <c r="Q324">
         <v>4</v>
       </c>
-      <c r="R324" s="12">
+      <c r="R324">
         <v>5</v>
       </c>
-      <c r="S324" s="12">
+      <c r="S324">
         <v>4</v>
       </c>
-      <c r="T324" s="12">
+      <c r="T324">
         <v>4</v>
       </c>
-      <c r="U324" s="12">
-        <v>0</v>
-      </c>
-      <c r="V324" s="12">
-        <v>0</v>
-      </c>
-      <c r="W324" s="12">
-        <v>0</v>
-      </c>
-      <c r="X324" s="12">
-        <v>0</v>
-      </c>
-      <c r="Y324" s="12">
+      <c r="U324">
+        <v>0</v>
+      </c>
+      <c r="V324">
+        <v>0</v>
+      </c>
+      <c r="W324">
+        <v>0</v>
+      </c>
+      <c r="X324">
+        <v>0</v>
+      </c>
+      <c r="Y324">
         <v>8</v>
       </c>
-      <c r="Z324" s="12">
-        <v>0</v>
-      </c>
-      <c r="AA324" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB324" s="12">
-        <v>0</v>
-      </c>
-      <c r="AC324" s="12">
-        <v>0</v>
-      </c>
-      <c r="AD324" s="12">
-        <v>2</v>
-      </c>
-      <c r="AE324" s="12">
-        <v>0</v>
-      </c>
-      <c r="AF324" s="12">
-        <v>0</v>
-      </c>
-      <c r="AG324" s="12">
-        <v>0</v>
-      </c>
-      <c r="AH324" s="12">
-        <v>0</v>
-      </c>
-      <c r="AI324" s="12">
-        <v>0</v>
-      </c>
-      <c r="AJ324" s="12">
-        <v>0</v>
-      </c>
-      <c r="AK324" s="12">
-        <v>1</v>
-      </c>
-      <c r="AL324" s="12">
-        <v>0</v>
-      </c>
-      <c r="AM324" s="12">
-        <v>0</v>
-      </c>
-      <c r="AN324" s="12">
-        <v>0</v>
-      </c>
-      <c r="AO324" s="12">
-        <v>0</v>
-      </c>
-      <c r="AP324" s="12">
-        <v>0</v>
-      </c>
-      <c r="AQ324" s="12">
-        <v>0</v>
-      </c>
-      <c r="AR324" s="12">
-        <v>0</v>
-      </c>
-      <c r="AS324" s="12">
-        <v>0</v>
-      </c>
-      <c r="AT324" s="12">
+      <c r="Z324">
+        <v>0</v>
+      </c>
+      <c r="AA324">
+        <v>0</v>
+      </c>
+      <c r="AB324">
+        <v>0</v>
+      </c>
+      <c r="AC324">
+        <v>0</v>
+      </c>
+      <c r="AD324">
+        <v>2</v>
+      </c>
+      <c r="AE324">
+        <v>0</v>
+      </c>
+      <c r="AF324">
+        <v>0</v>
+      </c>
+      <c r="AG324">
+        <v>0</v>
+      </c>
+      <c r="AH324">
+        <v>0</v>
+      </c>
+      <c r="AI324">
+        <v>0</v>
+      </c>
+      <c r="AJ324">
+        <v>0</v>
+      </c>
+      <c r="AK324">
+        <v>1</v>
+      </c>
+      <c r="AL324">
+        <v>0</v>
+      </c>
+      <c r="AM324">
+        <v>0</v>
+      </c>
+      <c r="AN324">
+        <v>0</v>
+      </c>
+      <c r="AO324">
+        <v>0</v>
+      </c>
+      <c r="AP324">
+        <v>0</v>
+      </c>
+      <c r="AQ324">
+        <v>0</v>
+      </c>
+      <c r="AR324">
+        <v>0</v>
+      </c>
+      <c r="AS324">
+        <v>0</v>
+      </c>
+      <c r="AT324">
         <v>0</v>
       </c>
     </row>
     <row r="325" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A325" s="12" t="s">
+      <c r="A325" t="s">
         <v>264</v>
       </c>
-      <c r="B325" s="13" t="s">
+      <c r="B325" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C325" s="14">
+      <c r="C325" s="4">
         <v>6.4</v>
       </c>
-      <c r="D325" s="12">
+      <c r="D325">
         <v>13</v>
       </c>
-      <c r="E325" s="12">
-        <v>0</v>
-      </c>
-      <c r="F325" s="12">
-        <v>0</v>
-      </c>
-      <c r="G325" s="12">
-        <v>0</v>
-      </c>
-      <c r="H325" s="12">
-        <v>0</v>
-      </c>
-      <c r="I325" s="12">
-        <v>0</v>
-      </c>
-      <c r="J325" s="12">
-        <v>0</v>
-      </c>
-      <c r="K325" s="12">
-        <v>0</v>
-      </c>
-      <c r="L325" s="12">
-        <v>0</v>
-      </c>
-      <c r="M325" s="12">
-        <v>0</v>
-      </c>
-      <c r="N325" s="12">
-        <v>0</v>
-      </c>
-      <c r="O325" s="12">
-        <v>0</v>
-      </c>
-      <c r="P325" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q325" s="12">
-        <v>2</v>
-      </c>
-      <c r="R325" s="12">
-        <v>3</v>
-      </c>
-      <c r="S325" s="12">
-        <v>0</v>
-      </c>
-      <c r="T325" s="12">
-        <v>1</v>
-      </c>
-      <c r="U325" s="12">
-        <v>2</v>
-      </c>
-      <c r="V325" s="12">
-        <v>2</v>
-      </c>
-      <c r="W325" s="12">
-        <v>0</v>
-      </c>
-      <c r="X325" s="12">
-        <v>0</v>
-      </c>
-      <c r="Y325" s="12">
+      <c r="E325">
+        <v>0</v>
+      </c>
+      <c r="F325">
+        <v>0</v>
+      </c>
+      <c r="G325">
+        <v>0</v>
+      </c>
+      <c r="H325">
+        <v>0</v>
+      </c>
+      <c r="I325">
+        <v>0</v>
+      </c>
+      <c r="J325">
+        <v>0</v>
+      </c>
+      <c r="K325">
+        <v>0</v>
+      </c>
+      <c r="L325">
+        <v>0</v>
+      </c>
+      <c r="M325">
+        <v>0</v>
+      </c>
+      <c r="N325">
+        <v>0</v>
+      </c>
+      <c r="O325">
+        <v>0</v>
+      </c>
+      <c r="P325">
+        <v>0</v>
+      </c>
+      <c r="Q325">
+        <v>2</v>
+      </c>
+      <c r="R325">
+        <v>3</v>
+      </c>
+      <c r="S325">
+        <v>0</v>
+      </c>
+      <c r="T325">
+        <v>1</v>
+      </c>
+      <c r="U325">
+        <v>2</v>
+      </c>
+      <c r="V325">
+        <v>2</v>
+      </c>
+      <c r="W325">
+        <v>0</v>
+      </c>
+      <c r="X325">
+        <v>0</v>
+      </c>
+      <c r="Y325">
         <v>4</v>
       </c>
-      <c r="Z325" s="12">
-        <v>1</v>
-      </c>
-      <c r="AA325" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB325" s="12">
-        <v>0</v>
-      </c>
-      <c r="AC325" s="12">
-        <v>0</v>
-      </c>
-      <c r="AD325" s="12">
-        <v>2</v>
-      </c>
-      <c r="AE325" s="12">
-        <v>0</v>
-      </c>
-      <c r="AF325" s="12">
-        <v>0</v>
-      </c>
-      <c r="AG325" s="12">
-        <v>0</v>
-      </c>
-      <c r="AH325" s="12">
-        <v>0</v>
-      </c>
-      <c r="AI325" s="12">
-        <v>0</v>
-      </c>
-      <c r="AJ325" s="12">
-        <v>0</v>
-      </c>
-      <c r="AK325" s="12">
-        <v>0</v>
-      </c>
-      <c r="AL325" s="12">
-        <v>0</v>
-      </c>
-      <c r="AM325" s="12">
-        <v>0</v>
-      </c>
-      <c r="AN325" s="12">
-        <v>0</v>
-      </c>
-      <c r="AO325" s="12">
-        <v>0</v>
-      </c>
-      <c r="AP325" s="12">
-        <v>0</v>
-      </c>
-      <c r="AQ325" s="12">
-        <v>0</v>
-      </c>
-      <c r="AR325" s="12">
-        <v>0</v>
-      </c>
-      <c r="AS325" s="12">
-        <v>0</v>
-      </c>
-      <c r="AT325" s="12">
+      <c r="Z325">
+        <v>1</v>
+      </c>
+      <c r="AA325">
+        <v>0</v>
+      </c>
+      <c r="AB325">
+        <v>0</v>
+      </c>
+      <c r="AC325">
+        <v>0</v>
+      </c>
+      <c r="AD325">
+        <v>2</v>
+      </c>
+      <c r="AE325">
+        <v>0</v>
+      </c>
+      <c r="AF325">
+        <v>0</v>
+      </c>
+      <c r="AG325">
+        <v>0</v>
+      </c>
+      <c r="AH325">
+        <v>0</v>
+      </c>
+      <c r="AI325">
+        <v>0</v>
+      </c>
+      <c r="AJ325">
+        <v>0</v>
+      </c>
+      <c r="AK325">
+        <v>0</v>
+      </c>
+      <c r="AL325">
+        <v>0</v>
+      </c>
+      <c r="AM325">
+        <v>0</v>
+      </c>
+      <c r="AN325">
+        <v>0</v>
+      </c>
+      <c r="AO325">
+        <v>0</v>
+      </c>
+      <c r="AP325">
+        <v>0</v>
+      </c>
+      <c r="AQ325">
+        <v>0</v>
+      </c>
+      <c r="AR325">
+        <v>0</v>
+      </c>
+      <c r="AS325">
+        <v>0</v>
+      </c>
+      <c r="AT325">
         <v>0</v>
       </c>
     </row>
@@ -53151,10 +53152,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4BDED69-97DE-43FA-AD0D-EB49DF8CFD17}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -53489,8 +53493,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>207</v>
+      <c r="A20">
+        <v>19</v>
       </c>
       <c r="B20" s="2">
         <v>45941</v>
@@ -53506,8 +53510,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>210</v>
+      <c r="A21">
+        <v>20</v>
       </c>
       <c r="B21" s="2">
         <v>45944</v>
@@ -53523,8 +53527,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>264</v>
+      <c r="A22">
+        <v>21</v>
       </c>
       <c r="B22" s="2">
         <v>45976</v>
@@ -53549,9 +53553,12 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35BA714C-9829-4B2A-B508-5AFF0D82E626}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
   <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
@@ -56762,8 +56769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A93F51-CDFA-4EA7-98BC-3EC790CF2226}">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Estructura de tablas completa
</commit_message>
<xml_diff>
--- a/data_raw/CONVOCATORIAS.xlsx
+++ b/data_raw/CONVOCATORIAS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OmarAndresMontanezMu\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67F0527-68A8-4CD2-A9ED-52DAEEE0860A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EC6B01-A29C-4979-AD42-5489491BD6F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{F7620B14-DF17-479D-BEA2-F7DF27FD67E6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{F7620B14-DF17-479D-BEA2-F7DF27FD67E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Convocatorias" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2163" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2112" uniqueCount="280">
   <si>
     <t>Jugador</t>
   </si>
@@ -664,16 +664,10 @@
     <t>Venezuela</t>
   </si>
   <si>
-    <t>Amistoso 1</t>
-  </si>
-  <si>
     <t>David Ospina</t>
   </si>
   <si>
     <t>Kevin Serna</t>
-  </si>
-  <si>
-    <t>Amistoso 2</t>
   </si>
   <si>
     <t>Canadá</t>
@@ -833,9 +827,6 @@
   </si>
   <si>
     <t>Racing de Santander</t>
-  </si>
-  <si>
-    <t>Amistoso 3</t>
   </si>
   <si>
     <t>Nueva Zelanda</t>
@@ -6693,7 +6684,7 @@
         <v>45933</v>
       </c>
       <c r="B275" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C275" s="4" t="s">
         <v>139</v>
@@ -6710,13 +6701,13 @@
         <v>45933</v>
       </c>
       <c r="B276" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C276" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D276" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E276" t="s">
         <v>120</v>
@@ -6727,7 +6718,7 @@
         <v>45933</v>
       </c>
       <c r="B277" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C277" s="4" t="s">
         <v>129</v>
@@ -6744,7 +6735,7 @@
         <v>45933</v>
       </c>
       <c r="B278" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C278" s="4" t="s">
         <v>17</v>
@@ -6761,7 +6752,7 @@
         <v>45933</v>
       </c>
       <c r="B279" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C279" s="4" t="s">
         <v>50</v>
@@ -6778,7 +6769,7 @@
         <v>45933</v>
       </c>
       <c r="B280" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C280" s="4" t="s">
         <v>18</v>
@@ -6795,7 +6786,7 @@
         <v>45933</v>
       </c>
       <c r="B281" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C281" s="4" t="s">
         <v>21</v>
@@ -6812,7 +6803,7 @@
         <v>45933</v>
       </c>
       <c r="B282" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C282" s="4" t="s">
         <v>48</v>
@@ -6829,7 +6820,7 @@
         <v>45933</v>
       </c>
       <c r="B283" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C283" s="4" t="s">
         <v>22</v>
@@ -6846,7 +6837,7 @@
         <v>45933</v>
       </c>
       <c r="B284" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C284" s="4" t="s">
         <v>26</v>
@@ -6863,7 +6854,7 @@
         <v>45933</v>
       </c>
       <c r="B285" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C285" s="4" t="s">
         <v>137</v>
@@ -6880,7 +6871,7 @@
         <v>45933</v>
       </c>
       <c r="B286" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C286" s="4" t="s">
         <v>27</v>
@@ -6897,13 +6888,13 @@
         <v>45933</v>
       </c>
       <c r="B287" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C287" s="4" t="s">
         <v>131</v>
       </c>
       <c r="D287" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E287" t="s">
         <v>119</v>
@@ -6914,7 +6905,7 @@
         <v>45933</v>
       </c>
       <c r="B288" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C288" s="4" t="s">
         <v>52</v>
@@ -6931,7 +6922,7 @@
         <v>45933</v>
       </c>
       <c r="B289" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C289" s="4" t="s">
         <v>29</v>
@@ -6948,7 +6939,7 @@
         <v>45933</v>
       </c>
       <c r="B290" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C290" s="4" t="s">
         <v>43</v>
@@ -6965,7 +6956,7 @@
         <v>45933</v>
       </c>
       <c r="B291" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C291" s="4" t="s">
         <v>44</v>
@@ -6982,10 +6973,10 @@
         <v>45933</v>
       </c>
       <c r="B292" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C292" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D292" t="s">
         <v>59</v>
@@ -6999,7 +6990,7 @@
         <v>45933</v>
       </c>
       <c r="B293" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C293" s="4" t="s">
         <v>31</v>
@@ -7016,7 +7007,7 @@
         <v>45933</v>
       </c>
       <c r="B294" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C294" s="4" t="s">
         <v>132</v>
@@ -7033,7 +7024,7 @@
         <v>45933</v>
       </c>
       <c r="B295" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C295" s="4" t="s">
         <v>35</v>
@@ -7050,7 +7041,7 @@
         <v>45933</v>
       </c>
       <c r="B296" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C296" s="4" t="s">
         <v>36</v>
@@ -7067,7 +7058,7 @@
         <v>45933</v>
       </c>
       <c r="B297" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C297" s="4" t="s">
         <v>46</v>
@@ -7084,7 +7075,7 @@
         <v>45933</v>
       </c>
       <c r="B298" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C298" s="6" t="s">
         <v>39</v>
@@ -7101,7 +7092,7 @@
         <v>45933</v>
       </c>
       <c r="B299" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C299" s="4" t="s">
         <v>47</v>
@@ -7118,7 +7109,7 @@
         <v>45933</v>
       </c>
       <c r="B300" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C300" s="5" t="s">
         <v>45</v>
@@ -7135,7 +7126,7 @@
         <v>45968</v>
       </c>
       <c r="B301" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C301" s="4" t="s">
         <v>15</v>
@@ -7152,7 +7143,7 @@
         <v>45968</v>
       </c>
       <c r="B302" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C302" s="4" t="s">
         <v>50</v>
@@ -7169,13 +7160,13 @@
         <v>45968</v>
       </c>
       <c r="B303" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C303" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D303" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E303" t="s">
         <v>120</v>
@@ -7186,7 +7177,7 @@
         <v>45968</v>
       </c>
       <c r="B304" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C304" s="4" t="s">
         <v>26</v>
@@ -7203,7 +7194,7 @@
         <v>45968</v>
       </c>
       <c r="B305" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C305" s="4" t="s">
         <v>17</v>
@@ -7220,13 +7211,13 @@
         <v>45968</v>
       </c>
       <c r="B306" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C306" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D306" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E306" t="s">
         <v>116</v>
@@ -7237,7 +7228,7 @@
         <v>45968</v>
       </c>
       <c r="B307" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C307" s="4" t="s">
         <v>39</v>
@@ -7254,7 +7245,7 @@
         <v>45968</v>
       </c>
       <c r="B308" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C308" s="4" t="s">
         <v>18</v>
@@ -7271,7 +7262,7 @@
         <v>45968</v>
       </c>
       <c r="B309" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C309" s="4" t="s">
         <v>37</v>
@@ -7288,7 +7279,7 @@
         <v>45968</v>
       </c>
       <c r="B310" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C310" s="4" t="s">
         <v>27</v>
@@ -7305,7 +7296,7 @@
         <v>45968</v>
       </c>
       <c r="B311" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C311" s="4" t="s">
         <v>139</v>
@@ -7322,7 +7313,7 @@
         <v>45968</v>
       </c>
       <c r="B312" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C312" s="4" t="s">
         <v>43</v>
@@ -7339,13 +7330,13 @@
         <v>45968</v>
       </c>
       <c r="B313" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C313" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D313" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E313" t="s">
         <v>116</v>
@@ -7356,13 +7347,13 @@
         <v>45968</v>
       </c>
       <c r="B314" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C314" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D314" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E314" t="s">
         <v>119</v>
@@ -7373,7 +7364,7 @@
         <v>45968</v>
       </c>
       <c r="B315" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C315" s="4" t="s">
         <v>21</v>
@@ -7390,7 +7381,7 @@
         <v>45968</v>
       </c>
       <c r="B316" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C316" s="4" t="s">
         <v>36</v>
@@ -7407,7 +7398,7 @@
         <v>45968</v>
       </c>
       <c r="B317" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C317" s="4" t="s">
         <v>22</v>
@@ -7424,7 +7415,7 @@
         <v>45968</v>
       </c>
       <c r="B318" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C318" s="4" t="s">
         <v>52</v>
@@ -7441,7 +7432,7 @@
         <v>45968</v>
       </c>
       <c r="B319" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C319" s="4" t="s">
         <v>23</v>
@@ -7458,7 +7449,7 @@
         <v>45968</v>
       </c>
       <c r="B320" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C320" s="4" t="s">
         <v>46</v>
@@ -7475,7 +7466,7 @@
         <v>45968</v>
       </c>
       <c r="B321" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C321" s="4" t="s">
         <v>31</v>
@@ -7492,7 +7483,7 @@
         <v>45968</v>
       </c>
       <c r="B322" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C322" s="4" t="s">
         <v>132</v>
@@ -7509,7 +7500,7 @@
         <v>45968</v>
       </c>
       <c r="B323" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C323" s="4" t="s">
         <v>35</v>
@@ -7526,7 +7517,7 @@
         <v>45968</v>
       </c>
       <c r="B324" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C324" s="4" t="s">
         <v>24</v>
@@ -7543,7 +7534,7 @@
         <v>45968</v>
       </c>
       <c r="B325" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C325" s="4" t="s">
         <v>137</v>
@@ -7560,13 +7551,13 @@
         <v>45968</v>
       </c>
       <c r="B326" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C326" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D326" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E326" t="s">
         <v>116</v>
@@ -7588,9 +7579,7 @@
   </sheetPr>
   <dimension ref="A1:AT325"/>
   <sheetViews>
-    <sheetView topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AT1" sqref="AT1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -46002,11 +45991,11 @@
       </c>
     </row>
     <row r="275" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A275" t="s">
+      <c r="A275">
+        <v>19</v>
+      </c>
+      <c r="B275" s="9" t="s">
         <v>207</v>
-      </c>
-      <c r="B275" s="9" t="s">
-        <v>208</v>
       </c>
       <c r="C275" s="4">
         <v>7.2</v>
@@ -46142,8 +46131,8 @@
       </c>
     </row>
     <row r="276" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A276" t="s">
-        <v>207</v>
+      <c r="A276">
+        <v>19</v>
       </c>
       <c r="B276" s="9" t="s">
         <v>17</v>
@@ -46282,8 +46271,8 @@
       </c>
     </row>
     <row r="277" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A277" t="s">
-        <v>207</v>
+      <c r="A277">
+        <v>19</v>
       </c>
       <c r="B277" s="9" t="s">
         <v>45</v>
@@ -46422,8 +46411,8 @@
       </c>
     </row>
     <row r="278" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A278" t="s">
-        <v>207</v>
+      <c r="A278">
+        <v>19</v>
       </c>
       <c r="B278" s="9" t="s">
         <v>26</v>
@@ -46562,8 +46551,8 @@
       </c>
     </row>
     <row r="279" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A279" t="s">
-        <v>207</v>
+      <c r="A279">
+        <v>19</v>
       </c>
       <c r="B279" s="9" t="s">
         <v>139</v>
@@ -46702,8 +46691,8 @@
       </c>
     </row>
     <row r="280" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A280" t="s">
-        <v>207</v>
+      <c r="A280">
+        <v>19</v>
       </c>
       <c r="B280" s="9" t="s">
         <v>22</v>
@@ -46842,8 +46831,8 @@
       </c>
     </row>
     <row r="281" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A281" t="s">
-        <v>207</v>
+      <c r="A281">
+        <v>19</v>
       </c>
       <c r="B281" s="9" t="s">
         <v>43</v>
@@ -46982,11 +46971,11 @@
       </c>
     </row>
     <row r="282" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A282" t="s">
-        <v>207</v>
+      <c r="A282">
+        <v>19</v>
       </c>
       <c r="B282" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C282" s="4">
         <v>6.7</v>
@@ -47122,8 +47111,8 @@
       </c>
     </row>
     <row r="283" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A283" t="s">
-        <v>207</v>
+      <c r="A283">
+        <v>19</v>
       </c>
       <c r="B283" s="9" t="s">
         <v>21</v>
@@ -47262,8 +47251,8 @@
       </c>
     </row>
     <row r="284" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A284" t="s">
-        <v>207</v>
+      <c r="A284">
+        <v>19</v>
       </c>
       <c r="B284" s="9" t="s">
         <v>164</v>
@@ -47402,8 +47391,8 @@
       </c>
     </row>
     <row r="285" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A285" t="s">
-        <v>207</v>
+      <c r="A285">
+        <v>19</v>
       </c>
       <c r="B285" s="9" t="s">
         <v>132</v>
@@ -47542,8 +47531,8 @@
       </c>
     </row>
     <row r="286" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A286" t="s">
-        <v>207</v>
+      <c r="A286">
+        <v>19</v>
       </c>
       <c r="B286" s="9" t="s">
         <v>48</v>
@@ -47682,8 +47671,8 @@
       </c>
     </row>
     <row r="287" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A287" t="s">
-        <v>207</v>
+      <c r="A287">
+        <v>19</v>
       </c>
       <c r="B287" s="9" t="s">
         <v>137</v>
@@ -47822,8 +47811,8 @@
       </c>
     </row>
     <row r="288" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A288" t="s">
-        <v>207</v>
+      <c r="A288">
+        <v>19</v>
       </c>
       <c r="B288" s="9" t="s">
         <v>29</v>
@@ -47962,8 +47951,8 @@
       </c>
     </row>
     <row r="289" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A289" t="s">
-        <v>207</v>
+      <c r="A289">
+        <v>19</v>
       </c>
       <c r="B289" s="9" t="s">
         <v>35</v>
@@ -48102,8 +48091,8 @@
       </c>
     </row>
     <row r="290" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A290" t="s">
-        <v>207</v>
+      <c r="A290">
+        <v>19</v>
       </c>
       <c r="B290" s="9" t="s">
         <v>52</v>
@@ -48242,8 +48231,8 @@
       </c>
     </row>
     <row r="291" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A291" t="s">
-        <v>207</v>
+      <c r="A291">
+        <v>19</v>
       </c>
       <c r="B291" s="9" t="s">
         <v>36</v>
@@ -48382,8 +48371,8 @@
       </c>
     </row>
     <row r="292" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A292" t="s">
-        <v>210</v>
+      <c r="A292">
+        <v>20</v>
       </c>
       <c r="B292" s="9" t="s">
         <v>14</v>
@@ -48522,8 +48511,8 @@
       </c>
     </row>
     <row r="293" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A293" t="s">
-        <v>210</v>
+      <c r="A293">
+        <v>20</v>
       </c>
       <c r="B293" s="9" t="s">
         <v>129</v>
@@ -48662,8 +48651,8 @@
       </c>
     </row>
     <row r="294" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A294" t="s">
-        <v>210</v>
+      <c r="A294">
+        <v>20</v>
       </c>
       <c r="B294" s="9" t="s">
         <v>18</v>
@@ -48802,8 +48791,8 @@
       </c>
     </row>
     <row r="295" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A295" t="s">
-        <v>210</v>
+      <c r="A295">
+        <v>20</v>
       </c>
       <c r="B295" s="9" t="s">
         <v>26</v>
@@ -48942,8 +48931,8 @@
       </c>
     </row>
     <row r="296" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A296" t="s">
-        <v>210</v>
+      <c r="A296">
+        <v>20</v>
       </c>
       <c r="B296" s="9" t="s">
         <v>27</v>
@@ -49082,8 +49071,8 @@
       </c>
     </row>
     <row r="297" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A297" t="s">
-        <v>210</v>
+      <c r="A297">
+        <v>20</v>
       </c>
       <c r="B297" s="9" t="s">
         <v>36</v>
@@ -49222,8 +49211,8 @@
       </c>
     </row>
     <row r="298" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A298" t="s">
-        <v>210</v>
+      <c r="A298">
+        <v>20</v>
       </c>
       <c r="B298" s="9" t="s">
         <v>52</v>
@@ -49362,8 +49351,8 @@
       </c>
     </row>
     <row r="299" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A299" t="s">
-        <v>210</v>
+      <c r="A299">
+        <v>20</v>
       </c>
       <c r="B299" s="9" t="s">
         <v>29</v>
@@ -49502,8 +49491,8 @@
       </c>
     </row>
     <row r="300" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A300" t="s">
-        <v>210</v>
+      <c r="A300">
+        <v>20</v>
       </c>
       <c r="B300" s="9" t="s">
         <v>48</v>
@@ -49642,8 +49631,8 @@
       </c>
     </row>
     <row r="301" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A301" t="s">
-        <v>210</v>
+      <c r="A301">
+        <v>20</v>
       </c>
       <c r="B301" s="9" t="s">
         <v>164</v>
@@ -49782,8 +49771,8 @@
       </c>
     </row>
     <row r="302" spans="1:46" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A302" t="s">
-        <v>210</v>
+      <c r="A302">
+        <v>20</v>
       </c>
       <c r="B302" s="9" t="s">
         <v>131</v>
@@ -49922,8 +49911,8 @@
       </c>
     </row>
     <row r="303" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A303" t="s">
-        <v>210</v>
+      <c r="A303">
+        <v>20</v>
       </c>
       <c r="B303" s="9" t="s">
         <v>21</v>
@@ -50062,11 +50051,11 @@
       </c>
     </row>
     <row r="304" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A304" t="s">
-        <v>210</v>
+      <c r="A304">
+        <v>20</v>
       </c>
       <c r="B304" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C304" s="4">
         <v>6.4</v>
@@ -50202,8 +50191,8 @@
       </c>
     </row>
     <row r="305" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A305" t="s">
-        <v>210</v>
+      <c r="A305">
+        <v>20</v>
       </c>
       <c r="B305" s="9" t="s">
         <v>46</v>
@@ -50342,8 +50331,8 @@
       </c>
     </row>
     <row r="306" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A306" t="s">
-        <v>210</v>
+      <c r="A306">
+        <v>20</v>
       </c>
       <c r="B306" s="9" t="s">
         <v>35</v>
@@ -50482,8 +50471,8 @@
       </c>
     </row>
     <row r="307" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A307" t="s">
-        <v>210</v>
+      <c r="A307">
+        <v>20</v>
       </c>
       <c r="B307" s="9" t="s">
         <v>43</v>
@@ -50622,8 +50611,8 @@
       </c>
     </row>
     <row r="308" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A308" t="s">
-        <v>210</v>
+      <c r="A308">
+        <v>20</v>
       </c>
       <c r="B308" s="9" t="s">
         <v>22</v>
@@ -50762,8 +50751,8 @@
       </c>
     </row>
     <row r="309" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A309" t="s">
-        <v>264</v>
+      <c r="A309">
+        <v>21</v>
       </c>
       <c r="B309" s="9" t="s">
         <v>14</v>
@@ -50902,8 +50891,8 @@
       </c>
     </row>
     <row r="310" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A310" t="s">
-        <v>264</v>
+      <c r="A310">
+        <v>21</v>
       </c>
       <c r="B310" s="9" t="s">
         <v>139</v>
@@ -51042,8 +51031,8 @@
       </c>
     </row>
     <row r="311" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A311" t="s">
-        <v>264</v>
+      <c r="A311">
+        <v>21</v>
       </c>
       <c r="B311" s="9" t="s">
         <v>16</v>
@@ -51182,8 +51171,8 @@
       </c>
     </row>
     <row r="312" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A312" t="s">
-        <v>264</v>
+      <c r="A312">
+        <v>21</v>
       </c>
       <c r="B312" s="9" t="s">
         <v>39</v>
@@ -51322,8 +51311,8 @@
       </c>
     </row>
     <row r="313" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A313" t="s">
-        <v>264</v>
+      <c r="A313">
+        <v>21</v>
       </c>
       <c r="B313" s="9" t="s">
         <v>37</v>
@@ -51462,8 +51451,8 @@
       </c>
     </row>
     <row r="314" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A314" t="s">
-        <v>264</v>
+      <c r="A314">
+        <v>21</v>
       </c>
       <c r="B314" s="9" t="s">
         <v>22</v>
@@ -51602,8 +51591,8 @@
       </c>
     </row>
     <row r="315" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A315" t="s">
-        <v>264</v>
+      <c r="A315">
+        <v>21</v>
       </c>
       <c r="B315" s="4" t="s">
         <v>51</v>
@@ -51742,8 +51731,8 @@
       </c>
     </row>
     <row r="316" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A316" t="s">
-        <v>264</v>
+      <c r="A316">
+        <v>21</v>
       </c>
       <c r="B316" s="9" t="s">
         <v>164</v>
@@ -51882,8 +51871,8 @@
       </c>
     </row>
     <row r="317" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A317" t="s">
-        <v>264</v>
+      <c r="A317">
+        <v>21</v>
       </c>
       <c r="B317" s="9" t="s">
         <v>21</v>
@@ -52022,8 +52011,8 @@
       </c>
     </row>
     <row r="318" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A318" t="s">
-        <v>264</v>
+      <c r="A318">
+        <v>21</v>
       </c>
       <c r="B318" s="9" t="s">
         <v>23</v>
@@ -52162,8 +52151,8 @@
       </c>
     </row>
     <row r="319" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A319" t="s">
-        <v>264</v>
+      <c r="A319">
+        <v>21</v>
       </c>
       <c r="B319" s="9" t="s">
         <v>24</v>
@@ -52302,8 +52291,8 @@
       </c>
     </row>
     <row r="320" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A320" t="s">
-        <v>264</v>
+      <c r="A320">
+        <v>21</v>
       </c>
       <c r="B320" s="9" t="s">
         <v>26</v>
@@ -52442,8 +52431,8 @@
       </c>
     </row>
     <row r="321" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A321" t="s">
-        <v>264</v>
+      <c r="A321">
+        <v>21</v>
       </c>
       <c r="B321" s="9" t="s">
         <v>43</v>
@@ -52582,8 +52571,8 @@
       </c>
     </row>
     <row r="322" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A322" t="s">
-        <v>264</v>
+      <c r="A322">
+        <v>21</v>
       </c>
       <c r="B322" s="9" t="s">
         <v>46</v>
@@ -52722,8 +52711,8 @@
       </c>
     </row>
     <row r="323" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A323" t="s">
-        <v>264</v>
+      <c r="A323">
+        <v>21</v>
       </c>
       <c r="B323" s="9" t="s">
         <v>28</v>
@@ -52862,8 +52851,8 @@
       </c>
     </row>
     <row r="324" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A324" t="s">
-        <v>264</v>
+      <c r="A324">
+        <v>21</v>
       </c>
       <c r="B324" s="9" t="s">
         <v>137</v>
@@ -53002,8 +52991,8 @@
       </c>
     </row>
     <row r="325" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A325" t="s">
-        <v>264</v>
+      <c r="A325">
+        <v>21</v>
       </c>
       <c r="B325" s="9" t="s">
         <v>35</v>
@@ -53157,7 +53146,7 @@
   </sheetPr>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -53174,16 +53163,16 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C1" t="s">
         <v>177</v>
       </c>
       <c r="D1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="E1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -53197,10 +53186,10 @@
         <v>206</v>
       </c>
       <c r="D2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -53214,10 +53203,10 @@
         <v>191</v>
       </c>
       <c r="D3" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E3" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -53231,10 +53220,10 @@
         <v>189</v>
       </c>
       <c r="D4" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -53248,10 +53237,10 @@
         <v>185</v>
       </c>
       <c r="D5" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E5" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -53265,10 +53254,10 @@
         <v>183</v>
       </c>
       <c r="D6" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -53282,10 +53271,10 @@
         <v>182</v>
       </c>
       <c r="D7" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E7" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -53299,10 +53288,10 @@
         <v>180</v>
       </c>
       <c r="D8" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -53316,10 +53305,10 @@
         <v>179</v>
       </c>
       <c r="D9" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -53333,10 +53322,10 @@
         <v>178</v>
       </c>
       <c r="D10" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E10" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -53350,10 +53339,10 @@
         <v>191</v>
       </c>
       <c r="D11" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -53367,10 +53356,10 @@
         <v>189</v>
       </c>
       <c r="D12" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -53384,10 +53373,10 @@
         <v>185</v>
       </c>
       <c r="D13" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -53401,10 +53390,10 @@
         <v>183</v>
       </c>
       <c r="D14" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -53418,10 +53407,10 @@
         <v>182</v>
       </c>
       <c r="D15" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -53435,10 +53424,10 @@
         <v>180</v>
       </c>
       <c r="D16" t="s">
+        <v>266</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>269</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -53452,10 +53441,10 @@
         <v>179</v>
       </c>
       <c r="D17" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -53469,10 +53458,10 @@
         <v>178</v>
       </c>
       <c r="D18" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -53486,10 +53475,10 @@
         <v>206</v>
       </c>
       <c r="D19" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -53500,13 +53489,13 @@
         <v>45941</v>
       </c>
       <c r="C20" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -53517,13 +53506,13 @@
         <v>45944</v>
       </c>
       <c r="C21" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D21" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -53534,13 +53523,13 @@
         <v>45976</v>
       </c>
       <c r="C22" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D22" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -53604,46 +53593,46 @@
         <v>161</v>
       </c>
       <c r="F1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H1" t="s">
+        <v>213</v>
+      </c>
+      <c r="I1" t="s">
+        <v>214</v>
+      </c>
+      <c r="J1" t="s">
         <v>215</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>216</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>217</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>218</v>
-      </c>
-      <c r="L1" t="s">
-        <v>219</v>
-      </c>
-      <c r="M1" t="s">
-        <v>220</v>
       </c>
       <c r="N1" t="s">
         <v>147</v>
       </c>
       <c r="O1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="P1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="Q1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="R1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -53657,13 +53646,13 @@
         <v>180</v>
       </c>
       <c r="D2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -53719,10 +53708,10 @@
         <v>173</v>
       </c>
       <c r="E3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -53763,10 +53752,10 @@
         <v>173</v>
       </c>
       <c r="E4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -53819,13 +53808,13 @@
         <v>185</v>
       </c>
       <c r="D5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -53866,10 +53855,10 @@
         <v>173</v>
       </c>
       <c r="E6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F6" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -53925,10 +53914,10 @@
         <v>173</v>
       </c>
       <c r="E7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -53981,13 +53970,13 @@
         <v>182</v>
       </c>
       <c r="D8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F8" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -54043,10 +54032,10 @@
         <v>173</v>
       </c>
       <c r="E9" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F9" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -54090,7 +54079,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B10">
         <v>37</v>
@@ -54102,10 +54091,10 @@
         <v>173</v>
       </c>
       <c r="E10" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F10" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -54146,10 +54135,10 @@
         <v>173</v>
       </c>
       <c r="E11" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F11" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -54208,7 +54197,7 @@
         <v>166</v>
       </c>
       <c r="F12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -54261,13 +54250,13 @@
         <v>179</v>
       </c>
       <c r="D13" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E13" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F13" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G13">
         <v>2</v>
@@ -54320,13 +54309,13 @@
         <v>174</v>
       </c>
       <c r="D14" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E14" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F14" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -54379,13 +54368,13 @@
         <v>180</v>
       </c>
       <c r="D15" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F15" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -54438,13 +54427,13 @@
         <v>168</v>
       </c>
       <c r="D16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F16" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G16">
         <v>3</v>
@@ -54503,7 +54492,7 @@
         <v>166</v>
       </c>
       <c r="F17" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -54559,10 +54548,10 @@
         <v>173</v>
       </c>
       <c r="E18" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F18" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -54621,7 +54610,7 @@
         <v>166</v>
       </c>
       <c r="F19" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -54674,13 +54663,13 @@
         <v>185</v>
       </c>
       <c r="D20" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E20" t="s">
         <v>166</v>
       </c>
       <c r="F20" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G20">
         <v>2</v>
@@ -54733,13 +54722,13 @@
         <v>185</v>
       </c>
       <c r="D21" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E21" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F21" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -54798,7 +54787,7 @@
         <v>166</v>
       </c>
       <c r="F22" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G22">
         <v>2</v>
@@ -54851,13 +54840,13 @@
         <v>185</v>
       </c>
       <c r="D23" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E23" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F23" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -54913,10 +54902,10 @@
         <v>173</v>
       </c>
       <c r="E24" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F24" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -54972,10 +54961,10 @@
         <v>173</v>
       </c>
       <c r="E25" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F25" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -55031,10 +55020,10 @@
         <v>173</v>
       </c>
       <c r="E26" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F26" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -55087,13 +55076,13 @@
         <v>185</v>
       </c>
       <c r="D27" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E27" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F27" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G27">
         <v>1</v>
@@ -55146,13 +55135,13 @@
         <v>168</v>
       </c>
       <c r="D28" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E28" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F28" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -55208,10 +55197,10 @@
         <v>173</v>
       </c>
       <c r="E29" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F29" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G29">
         <v>5</v>
@@ -55267,10 +55256,10 @@
         <v>173</v>
       </c>
       <c r="E30" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F30" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -55326,10 +55315,10 @@
         <v>173</v>
       </c>
       <c r="E31" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F31" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -55358,7 +55347,7 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B32">
         <v>27</v>
@@ -55370,10 +55359,10 @@
         <v>173</v>
       </c>
       <c r="E32" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F32" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -55432,7 +55421,7 @@
         <v>166</v>
       </c>
       <c r="F33" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -55491,7 +55480,7 @@
         <v>166</v>
       </c>
       <c r="F34" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G34">
         <v>3</v>
@@ -55550,7 +55539,7 @@
         <v>166</v>
       </c>
       <c r="F35" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -55606,10 +55595,10 @@
         <v>173</v>
       </c>
       <c r="E36" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F36" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -55665,10 +55654,10 @@
         <v>173</v>
       </c>
       <c r="E37" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F37" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G37">
         <v>2</v>
@@ -55724,10 +55713,10 @@
         <v>173</v>
       </c>
       <c r="E38" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F38" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -55786,7 +55775,7 @@
         <v>166</v>
       </c>
       <c r="F39" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G39">
         <v>4</v>
@@ -55842,10 +55831,10 @@
         <v>173</v>
       </c>
       <c r="E40" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F40" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G40">
         <v>1</v>
@@ -55904,7 +55893,7 @@
         <v>166</v>
       </c>
       <c r="F41" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -55960,10 +55949,10 @@
         <v>173</v>
       </c>
       <c r="E42" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F42" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G42">
         <v>1</v>
@@ -56019,10 +56008,10 @@
         <v>173</v>
       </c>
       <c r="E43" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F43" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -56078,10 +56067,10 @@
         <v>173</v>
       </c>
       <c r="E44" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F44" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -56134,13 +56123,13 @@
         <v>176</v>
       </c>
       <c r="D45" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E45" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F45" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -56196,10 +56185,10 @@
         <v>173</v>
       </c>
       <c r="E46" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F46" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G46">
         <v>3</v>
@@ -56255,10 +56244,10 @@
         <v>173</v>
       </c>
       <c r="E47" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F47" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -56314,10 +56303,10 @@
         <v>173</v>
       </c>
       <c r="E48" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F48" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -56361,7 +56350,7 @@
         <v>166</v>
       </c>
       <c r="F49" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G49">
         <v>1</v>
@@ -56417,10 +56406,10 @@
         <v>173</v>
       </c>
       <c r="E50" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F50" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G50">
         <v>0</v>
@@ -56479,7 +56468,7 @@
         <v>166</v>
       </c>
       <c r="F51" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G51">
         <v>1</v>
@@ -56535,10 +56524,10 @@
         <v>173</v>
       </c>
       <c r="E52" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F52" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G52">
         <v>0</v>
@@ -56591,13 +56580,13 @@
         <v>185</v>
       </c>
       <c r="D53" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E53" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F53" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G53">
         <v>1</v>
@@ -56653,10 +56642,10 @@
         <v>173</v>
       </c>
       <c r="E54" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F54" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -56709,13 +56698,13 @@
         <v>172</v>
       </c>
       <c r="D55" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E55" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F55" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -56786,40 +56775,40 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E1" t="s">
+        <v>231</v>
+      </c>
+      <c r="F1" t="s">
         <v>232</v>
       </c>
-      <c r="C1" t="s">
-        <v>230</v>
-      </c>
-      <c r="D1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>233</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>234</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>235</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>236</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>237</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>238</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>239</v>
-      </c>
-      <c r="L1" t="s">
-        <v>240</v>
-      </c>
-      <c r="M1" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -57521,7 +57510,7 @@
     </row>
     <row r="19" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B19">
         <v>7.1</v>
@@ -58505,7 +58494,7 @@
     </row>
     <row r="43" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B43">
         <v>7</v>
@@ -59064,40 +59053,40 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E1" t="s">
+        <v>231</v>
+      </c>
+      <c r="F1" t="s">
         <v>232</v>
       </c>
-      <c r="C1" t="s">
-        <v>230</v>
-      </c>
-      <c r="D1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>233</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>234</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>235</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>236</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>237</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>238</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>239</v>
-      </c>
-      <c r="L1" t="s">
-        <v>240</v>
-      </c>
-      <c r="M1" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -59799,7 +59788,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B19">
         <v>3</v>
@@ -60783,7 +60772,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B43">
         <v>5</v>

</xml_diff>